<commit_message>
add line 5 to mapping
</commit_message>
<xml_diff>
--- a/src/statuscode_led_mapping_template.xlsx
+++ b/src/statuscode_led_mapping_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robin\Documents\github\rnv-train-monitor\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D87584D-9C44-4F12-BBA3-E3A271B83167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F1F2C-5F48-4521-850C-724A718D700F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{6BC448DE-82B4-40A0-A0A8-5C16E427463C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="250">
   <si>
     <t>statuscode</t>
   </si>
@@ -720,6 +720,69 @@
   </si>
   <si>
     <t>Stadtwerke</t>
+  </si>
+  <si>
+    <t>5 D-E transit</t>
+  </si>
+  <si>
+    <t>5 E-D transit</t>
+  </si>
+  <si>
+    <t>5 E-D stopped</t>
+  </si>
+  <si>
+    <t>5 D-E stopped</t>
+  </si>
+  <si>
+    <t>5 D-E stopped last</t>
+  </si>
+  <si>
+    <t>5 E-D stopped last</t>
+  </si>
+  <si>
+    <t>5 D-E stopped first</t>
+  </si>
+  <si>
+    <t>5 E-D stopped first</t>
+  </si>
+  <si>
+    <t>Dossenheim Nord &gt; Dossenheim Bf</t>
+  </si>
+  <si>
+    <t>Wieblingen Taubenfeld &gt; Edingen Bahnhof</t>
+  </si>
+  <si>
+    <t>Edingen Bahnhof &gt; Wieblingen Taubenfeld</t>
+  </si>
+  <si>
+    <t>Dossenheim Bf</t>
+  </si>
+  <si>
+    <t>Taubenfeld</t>
+  </si>
+  <si>
+    <t>Edingen Bahnhof</t>
+  </si>
+  <si>
+    <t>Dossenheim Nord</t>
+  </si>
+  <si>
+    <t>Burgstraße &gt; Hans Thoma</t>
+  </si>
+  <si>
+    <t>Hans Thoma &gt; Burgstraße</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burgstraße  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hans Thoma  </t>
+  </si>
+  <si>
+    <t>Hans Thoma</t>
+  </si>
+  <si>
+    <t>Burgstraße</t>
   </si>
 </sst>
 </file>
@@ -1587,11 +1650,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049D7F86-3D4A-4BAF-A7FA-ECA534A64199}">
-  <dimension ref="A1:Q422"/>
+  <dimension ref="A1:Q580"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
+      <pane ySplit="1" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D587" sqref="D587"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,6 +1663,7 @@
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
     <col min="16" max="16" width="28.28515625" customWidth="1"/>
     <col min="17" max="17" width="20" customWidth="1"/>
   </cols>
@@ -13046,13 +13110,13 @@
         <v>118722</v>
       </c>
     </row>
-    <row r="417" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A417" t="str">
         <f t="shared" si="13"/>
         <v>114423_116023_DEPOT</v>
       </c>
       <c r="B417" t="str">
-        <f t="shared" ref="B417:B422" si="15">_xlfn.CONCAT(G417,"-",H417)</f>
+        <f t="shared" ref="B417:B466" si="15">_xlfn.CONCAT(G417,"-",H417)</f>
         <v>36-20</v>
       </c>
       <c r="C417" t="s">
@@ -13077,7 +13141,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="418" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A418" t="str">
         <f t="shared" si="13"/>
         <v>116023_119421_DEPOT</v>
@@ -13105,7 +13169,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="419" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A419" t="str">
         <f t="shared" si="13"/>
         <v>119421_118722_DEPOT</v>
@@ -13136,7 +13200,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="420" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A420" t="str">
         <f t="shared" si="13"/>
         <v>DEPOT_114423_116023</v>
@@ -13167,7 +13231,7 @@
         <v>116023</v>
       </c>
     </row>
-    <row r="421" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A421" t="str">
         <f t="shared" si="13"/>
         <v>DEPOT_116023_119421</v>
@@ -13195,7 +13259,7 @@
         <v>119421</v>
       </c>
     </row>
-    <row r="422" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A422" t="str">
         <f t="shared" si="13"/>
         <v>DEPOT_119421_118722</v>
@@ -13224,6 +13288,4490 @@
       </c>
       <c r="M422">
         <v>118722</v>
+      </c>
+    </row>
+    <row r="423" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A423" t="str">
+        <f t="shared" ref="A423:A462" si="16">_xlfn.CONCAT(K423,"_",M423)</f>
+        <v>574201_51501</v>
+      </c>
+      <c r="B423" t="str">
+        <f t="shared" si="15"/>
+        <v>61-24</v>
+      </c>
+      <c r="C423" t="s">
+        <v>229</v>
+      </c>
+      <c r="D423" t="s">
+        <v>237</v>
+      </c>
+      <c r="G423">
+        <v>61</v>
+      </c>
+      <c r="H423">
+        <v>24</v>
+      </c>
+      <c r="K423">
+        <v>574201</v>
+      </c>
+      <c r="M423">
+        <v>51501</v>
+      </c>
+      <c r="P423">
+        <v>51601</v>
+      </c>
+      <c r="Q423">
+        <v>130201</v>
+      </c>
+    </row>
+    <row r="424" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A424" t="str">
+        <f t="shared" si="16"/>
+        <v>51501_51601</v>
+      </c>
+      <c r="B424" t="str">
+        <f t="shared" si="15"/>
+        <v>59-24</v>
+      </c>
+      <c r="C424" t="s">
+        <v>229</v>
+      </c>
+      <c r="G424">
+        <v>59</v>
+      </c>
+      <c r="H424">
+        <v>24</v>
+      </c>
+      <c r="K424">
+        <v>51501</v>
+      </c>
+      <c r="M424">
+        <v>51601</v>
+      </c>
+      <c r="P424">
+        <v>113301</v>
+      </c>
+      <c r="Q424">
+        <v>169301</v>
+      </c>
+    </row>
+    <row r="425" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A425" t="str">
+        <f t="shared" si="16"/>
+        <v>51601_113301</v>
+      </c>
+      <c r="B425" t="str">
+        <f t="shared" si="15"/>
+        <v>57-24</v>
+      </c>
+      <c r="C425" t="s">
+        <v>229</v>
+      </c>
+      <c r="G425">
+        <v>57</v>
+      </c>
+      <c r="H425">
+        <v>24</v>
+      </c>
+      <c r="K425">
+        <v>51601</v>
+      </c>
+      <c r="M425">
+        <v>113301</v>
+      </c>
+      <c r="P425">
+        <v>113601</v>
+      </c>
+      <c r="Q425">
+        <v>118001</v>
+      </c>
+    </row>
+    <row r="426" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A426" t="str">
+        <f t="shared" si="16"/>
+        <v>113301_113601</v>
+      </c>
+      <c r="B426" t="str">
+        <f t="shared" si="15"/>
+        <v>55-24</v>
+      </c>
+      <c r="C426" t="s">
+        <v>229</v>
+      </c>
+      <c r="D426" t="s">
+        <v>244</v>
+      </c>
+      <c r="G426">
+        <v>55</v>
+      </c>
+      <c r="H426">
+        <v>24</v>
+      </c>
+      <c r="K426">
+        <v>113301</v>
+      </c>
+      <c r="M426">
+        <v>113601</v>
+      </c>
+      <c r="P426">
+        <v>113521</v>
+      </c>
+      <c r="Q426">
+        <v>133101</v>
+      </c>
+    </row>
+    <row r="427" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A427" t="str">
+        <f t="shared" si="16"/>
+        <v>113601_113521</v>
+      </c>
+      <c r="B427" t="str">
+        <f t="shared" si="15"/>
+        <v>51-24</v>
+      </c>
+      <c r="C427" t="s">
+        <v>229</v>
+      </c>
+      <c r="G427">
+        <v>51</v>
+      </c>
+      <c r="H427">
+        <v>24</v>
+      </c>
+      <c r="K427">
+        <v>113601</v>
+      </c>
+      <c r="M427">
+        <v>113521</v>
+      </c>
+      <c r="P427">
+        <v>122521</v>
+      </c>
+      <c r="Q427">
+        <v>133001</v>
+      </c>
+    </row>
+    <row r="428" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A428" t="str">
+        <f t="shared" si="16"/>
+        <v>113521_122521</v>
+      </c>
+      <c r="B428" t="str">
+        <f t="shared" si="15"/>
+        <v>47-27</v>
+      </c>
+      <c r="C428" t="s">
+        <v>229</v>
+      </c>
+      <c r="G428">
+        <v>47</v>
+      </c>
+      <c r="H428">
+        <v>27</v>
+      </c>
+      <c r="K428">
+        <v>113521</v>
+      </c>
+      <c r="M428">
+        <v>122521</v>
+      </c>
+      <c r="P428">
+        <v>123321</v>
+      </c>
+      <c r="Q428">
+        <v>116021</v>
+      </c>
+    </row>
+    <row r="429" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A429" t="str">
+        <f t="shared" si="16"/>
+        <v>122521_123321</v>
+      </c>
+      <c r="B429" t="str">
+        <f t="shared" si="15"/>
+        <v>45-29</v>
+      </c>
+      <c r="C429" t="s">
+        <v>229</v>
+      </c>
+      <c r="G429">
+        <v>45</v>
+      </c>
+      <c r="H429">
+        <v>29</v>
+      </c>
+      <c r="K429">
+        <v>122521</v>
+      </c>
+      <c r="M429">
+        <v>123321</v>
+      </c>
+      <c r="P429">
+        <v>126021</v>
+      </c>
+      <c r="Q429">
+        <v>119421</v>
+      </c>
+    </row>
+    <row r="430" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A430" t="str">
+        <f t="shared" si="16"/>
+        <v>123321_126021</v>
+      </c>
+      <c r="B430" t="str">
+        <f t="shared" si="15"/>
+        <v>43-29</v>
+      </c>
+      <c r="C430" t="s">
+        <v>229</v>
+      </c>
+      <c r="G430">
+        <v>43</v>
+      </c>
+      <c r="H430">
+        <v>29</v>
+      </c>
+      <c r="K430">
+        <v>123321</v>
+      </c>
+      <c r="M430">
+        <v>126021</v>
+      </c>
+      <c r="P430">
+        <v>114602</v>
+      </c>
+      <c r="Q430">
+        <v>119321</v>
+      </c>
+    </row>
+    <row r="431" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A431" t="str">
+        <f t="shared" si="16"/>
+        <v>126021_114602</v>
+      </c>
+      <c r="B431" t="str">
+        <f t="shared" si="15"/>
+        <v>41-29</v>
+      </c>
+      <c r="C431" t="s">
+        <v>229</v>
+      </c>
+      <c r="G431">
+        <v>41</v>
+      </c>
+      <c r="H431">
+        <v>29</v>
+      </c>
+      <c r="K431">
+        <v>126021</v>
+      </c>
+      <c r="M431">
+        <v>114602</v>
+      </c>
+      <c r="P431">
+        <v>116822</v>
+      </c>
+      <c r="Q431">
+        <v>116821</v>
+      </c>
+    </row>
+    <row r="432" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A432" t="str">
+        <f t="shared" si="16"/>
+        <v>114602_116822</v>
+      </c>
+      <c r="B432" t="str">
+        <f t="shared" si="15"/>
+        <v>38-29</v>
+      </c>
+      <c r="C432" t="s">
+        <v>229</v>
+      </c>
+      <c r="G432">
+        <v>38</v>
+      </c>
+      <c r="H432">
+        <v>29</v>
+      </c>
+      <c r="K432">
+        <v>114602</v>
+      </c>
+      <c r="M432">
+        <v>116822</v>
+      </c>
+      <c r="P432">
+        <v>119322</v>
+      </c>
+      <c r="Q432">
+        <v>114601</v>
+      </c>
+    </row>
+    <row r="433" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A433" t="str">
+        <f t="shared" si="16"/>
+        <v>116822_119322</v>
+      </c>
+      <c r="B433" t="str">
+        <f t="shared" si="15"/>
+        <v>37-27</v>
+      </c>
+      <c r="C433" t="s">
+        <v>229</v>
+      </c>
+      <c r="G433">
+        <v>37</v>
+      </c>
+      <c r="H433">
+        <v>27</v>
+      </c>
+      <c r="K433">
+        <v>116822</v>
+      </c>
+      <c r="M433">
+        <v>119322</v>
+      </c>
+      <c r="P433">
+        <v>119402</v>
+      </c>
+      <c r="Q433">
+        <v>126022</v>
+      </c>
+    </row>
+    <row r="434" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A434" t="str">
+        <f t="shared" si="16"/>
+        <v>119322_119402</v>
+      </c>
+      <c r="B434" t="str">
+        <f t="shared" si="15"/>
+        <v>37-25</v>
+      </c>
+      <c r="C434" t="s">
+        <v>229</v>
+      </c>
+      <c r="G434">
+        <v>37</v>
+      </c>
+      <c r="H434">
+        <v>25</v>
+      </c>
+      <c r="K434">
+        <v>119322</v>
+      </c>
+      <c r="M434">
+        <v>119402</v>
+      </c>
+      <c r="P434">
+        <v>116022</v>
+      </c>
+      <c r="Q434">
+        <v>123322</v>
+      </c>
+    </row>
+    <row r="435" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A435" t="str">
+        <f t="shared" si="16"/>
+        <v>119402_116022</v>
+      </c>
+      <c r="B435" t="str">
+        <f t="shared" si="15"/>
+        <v>37-21</v>
+      </c>
+      <c r="C435" t="s">
+        <v>229</v>
+      </c>
+      <c r="G435">
+        <v>37</v>
+      </c>
+      <c r="H435">
+        <v>21</v>
+      </c>
+      <c r="K435">
+        <v>119402</v>
+      </c>
+      <c r="M435">
+        <v>116022</v>
+      </c>
+      <c r="P435">
+        <v>133002</v>
+      </c>
+      <c r="Q435">
+        <v>122522</v>
+      </c>
+    </row>
+    <row r="436" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A436" t="str">
+        <f t="shared" si="16"/>
+        <v>116022_133002</v>
+      </c>
+      <c r="B436" t="str">
+        <f t="shared" si="15"/>
+        <v>37-18</v>
+      </c>
+      <c r="C436" t="s">
+        <v>229</v>
+      </c>
+      <c r="G436">
+        <v>37</v>
+      </c>
+      <c r="H436">
+        <v>18</v>
+      </c>
+      <c r="K436">
+        <v>116022</v>
+      </c>
+      <c r="M436">
+        <v>133002</v>
+      </c>
+      <c r="P436">
+        <v>133102</v>
+      </c>
+      <c r="Q436">
+        <v>113522</v>
+      </c>
+    </row>
+    <row r="437" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A437" t="str">
+        <f t="shared" si="16"/>
+        <v>133002_133102</v>
+      </c>
+      <c r="B437" t="str">
+        <f t="shared" si="15"/>
+        <v>40-14</v>
+      </c>
+      <c r="C437" t="s">
+        <v>229</v>
+      </c>
+      <c r="G437">
+        <v>40</v>
+      </c>
+      <c r="H437">
+        <v>14</v>
+      </c>
+      <c r="K437">
+        <v>133002</v>
+      </c>
+      <c r="M437">
+        <v>133102</v>
+      </c>
+      <c r="P437">
+        <v>118002</v>
+      </c>
+      <c r="Q437">
+        <v>113602</v>
+      </c>
+    </row>
+    <row r="438" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A438" t="str">
+        <f t="shared" si="16"/>
+        <v>133102_118002</v>
+      </c>
+      <c r="B438" t="str">
+        <f t="shared" si="15"/>
+        <v>42-12</v>
+      </c>
+      <c r="C438" t="s">
+        <v>229</v>
+      </c>
+      <c r="G438">
+        <v>42</v>
+      </c>
+      <c r="H438">
+        <v>12</v>
+      </c>
+      <c r="K438">
+        <v>133102</v>
+      </c>
+      <c r="M438">
+        <v>118002</v>
+      </c>
+      <c r="P438">
+        <v>169302</v>
+      </c>
+      <c r="Q438">
+        <v>113302</v>
+      </c>
+    </row>
+    <row r="439" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A439" t="str">
+        <f t="shared" si="16"/>
+        <v>118002_169302</v>
+      </c>
+      <c r="B439" t="str">
+        <f t="shared" si="15"/>
+        <v>44-10</v>
+      </c>
+      <c r="C439" t="s">
+        <v>229</v>
+      </c>
+      <c r="G439">
+        <v>44</v>
+      </c>
+      <c r="H439">
+        <v>10</v>
+      </c>
+      <c r="K439">
+        <v>118002</v>
+      </c>
+      <c r="M439">
+        <v>169302</v>
+      </c>
+      <c r="P439">
+        <v>130202</v>
+      </c>
+      <c r="Q439">
+        <v>51602</v>
+      </c>
+    </row>
+    <row r="440" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A440" t="str">
+        <f t="shared" si="16"/>
+        <v>169302_130202</v>
+      </c>
+      <c r="B440" t="str">
+        <f t="shared" si="15"/>
+        <v>46-8</v>
+      </c>
+      <c r="C440" t="s">
+        <v>229</v>
+      </c>
+      <c r="G440">
+        <v>46</v>
+      </c>
+      <c r="H440">
+        <v>8</v>
+      </c>
+      <c r="K440">
+        <v>169302</v>
+      </c>
+      <c r="M440">
+        <v>130202</v>
+      </c>
+      <c r="P440">
+        <v>130402</v>
+      </c>
+      <c r="Q440">
+        <v>51502</v>
+      </c>
+    </row>
+    <row r="441" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A441" t="str">
+        <f t="shared" si="16"/>
+        <v>130202_130402</v>
+      </c>
+      <c r="B441" t="str">
+        <f t="shared" si="15"/>
+        <v>48-6</v>
+      </c>
+      <c r="C441" t="s">
+        <v>229</v>
+      </c>
+      <c r="G441">
+        <v>48</v>
+      </c>
+      <c r="H441">
+        <v>6</v>
+      </c>
+      <c r="K441">
+        <v>130202</v>
+      </c>
+      <c r="M441">
+        <v>130402</v>
+      </c>
+      <c r="P441">
+        <v>61901</v>
+      </c>
+      <c r="Q441">
+        <v>574202</v>
+      </c>
+    </row>
+    <row r="442" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A442" t="str">
+        <f t="shared" si="16"/>
+        <v>130402_61901</v>
+      </c>
+      <c r="B442" t="str">
+        <f t="shared" si="15"/>
+        <v>50-3</v>
+      </c>
+      <c r="C442" t="s">
+        <v>229</v>
+      </c>
+      <c r="D442" t="s">
+        <v>238</v>
+      </c>
+      <c r="G442">
+        <v>50</v>
+      </c>
+      <c r="H442">
+        <v>3</v>
+      </c>
+      <c r="K442">
+        <v>130402</v>
+      </c>
+      <c r="M442">
+        <v>61901</v>
+      </c>
+    </row>
+    <row r="443" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A443" t="str">
+        <f t="shared" si="16"/>
+        <v>61902_130401</v>
+      </c>
+      <c r="B443" t="str">
+        <f t="shared" si="15"/>
+        <v>49-3</v>
+      </c>
+      <c r="C443" t="s">
+        <v>230</v>
+      </c>
+      <c r="D443" t="s">
+        <v>239</v>
+      </c>
+      <c r="G443">
+        <v>49</v>
+      </c>
+      <c r="H443">
+        <v>3</v>
+      </c>
+      <c r="K443">
+        <v>61902</v>
+      </c>
+      <c r="M443">
+        <v>130401</v>
+      </c>
+    </row>
+    <row r="444" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A444" t="str">
+        <f t="shared" si="16"/>
+        <v>130401_130201</v>
+      </c>
+      <c r="B444" t="str">
+        <f t="shared" si="15"/>
+        <v>47-5</v>
+      </c>
+      <c r="C444" t="s">
+        <v>230</v>
+      </c>
+      <c r="G444">
+        <v>47</v>
+      </c>
+      <c r="H444">
+        <v>5</v>
+      </c>
+      <c r="K444">
+        <v>130401</v>
+      </c>
+      <c r="M444">
+        <v>130201</v>
+      </c>
+    </row>
+    <row r="445" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A445" t="str">
+        <f t="shared" si="16"/>
+        <v>130201_169301</v>
+      </c>
+      <c r="B445" t="str">
+        <f t="shared" si="15"/>
+        <v>45-7</v>
+      </c>
+      <c r="C445" t="s">
+        <v>230</v>
+      </c>
+      <c r="G445">
+        <v>45</v>
+      </c>
+      <c r="H445">
+        <v>7</v>
+      </c>
+      <c r="K445">
+        <v>130201</v>
+      </c>
+      <c r="M445">
+        <v>169301</v>
+      </c>
+    </row>
+    <row r="446" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A446" t="str">
+        <f t="shared" si="16"/>
+        <v>169301_118001</v>
+      </c>
+      <c r="B446" t="str">
+        <f t="shared" si="15"/>
+        <v>43-9</v>
+      </c>
+      <c r="C446" t="s">
+        <v>230</v>
+      </c>
+      <c r="G446">
+        <v>43</v>
+      </c>
+      <c r="H446">
+        <v>9</v>
+      </c>
+      <c r="K446">
+        <v>169301</v>
+      </c>
+      <c r="M446">
+        <v>118001</v>
+      </c>
+    </row>
+    <row r="447" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A447" t="str">
+        <f t="shared" si="16"/>
+        <v>118001_133101</v>
+      </c>
+      <c r="B447" t="str">
+        <f t="shared" si="15"/>
+        <v>41-11</v>
+      </c>
+      <c r="C447" t="s">
+        <v>230</v>
+      </c>
+      <c r="G447">
+        <v>41</v>
+      </c>
+      <c r="H447">
+        <v>11</v>
+      </c>
+      <c r="K447">
+        <v>118001</v>
+      </c>
+      <c r="M447">
+        <v>133101</v>
+      </c>
+    </row>
+    <row r="448" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A448" t="str">
+        <f t="shared" si="16"/>
+        <v>133101_133001</v>
+      </c>
+      <c r="B448" t="str">
+        <f t="shared" si="15"/>
+        <v>39-13</v>
+      </c>
+      <c r="C448" t="s">
+        <v>230</v>
+      </c>
+      <c r="G448">
+        <v>39</v>
+      </c>
+      <c r="H448">
+        <v>13</v>
+      </c>
+      <c r="K448">
+        <v>133101</v>
+      </c>
+      <c r="M448">
+        <v>133001</v>
+      </c>
+    </row>
+    <row r="449" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A449" t="str">
+        <f t="shared" si="16"/>
+        <v>133001_116021</v>
+      </c>
+      <c r="B449" t="str">
+        <f t="shared" si="15"/>
+        <v>36-18</v>
+      </c>
+      <c r="C449" t="s">
+        <v>230</v>
+      </c>
+      <c r="G449">
+        <v>36</v>
+      </c>
+      <c r="H449">
+        <v>18</v>
+      </c>
+      <c r="K449">
+        <v>133001</v>
+      </c>
+      <c r="M449">
+        <v>116021</v>
+      </c>
+    </row>
+    <row r="450" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A450" t="str">
+        <f t="shared" si="16"/>
+        <v>116021_119421</v>
+      </c>
+      <c r="B450" t="str">
+        <f t="shared" si="15"/>
+        <v>36-21</v>
+      </c>
+      <c r="C450" t="s">
+        <v>230</v>
+      </c>
+      <c r="G450">
+        <v>36</v>
+      </c>
+      <c r="H450">
+        <v>21</v>
+      </c>
+      <c r="K450">
+        <v>116021</v>
+      </c>
+      <c r="M450">
+        <v>119421</v>
+      </c>
+    </row>
+    <row r="451" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A451" t="str">
+        <f t="shared" si="16"/>
+        <v>119421_119321</v>
+      </c>
+      <c r="B451" t="str">
+        <f t="shared" si="15"/>
+        <v>36-23</v>
+      </c>
+      <c r="C451" t="s">
+        <v>230</v>
+      </c>
+      <c r="G451">
+        <v>36</v>
+      </c>
+      <c r="H451">
+        <v>23</v>
+      </c>
+      <c r="K451">
+        <v>119421</v>
+      </c>
+      <c r="M451">
+        <v>119321</v>
+      </c>
+    </row>
+    <row r="452" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A452" t="str">
+        <f t="shared" si="16"/>
+        <v>119321_116821</v>
+      </c>
+      <c r="B452" t="str">
+        <f t="shared" si="15"/>
+        <v>36-27</v>
+      </c>
+      <c r="C452" t="s">
+        <v>230</v>
+      </c>
+      <c r="G452">
+        <v>36</v>
+      </c>
+      <c r="H452">
+        <v>27</v>
+      </c>
+      <c r="K452">
+        <v>119321</v>
+      </c>
+      <c r="M452">
+        <v>116821</v>
+      </c>
+    </row>
+    <row r="453" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A453" t="str">
+        <f t="shared" si="16"/>
+        <v>116821_114601</v>
+      </c>
+      <c r="B453" t="str">
+        <f t="shared" si="15"/>
+        <v>38-30</v>
+      </c>
+      <c r="C453" t="s">
+        <v>230</v>
+      </c>
+      <c r="G453">
+        <v>38</v>
+      </c>
+      <c r="H453">
+        <v>30</v>
+      </c>
+      <c r="K453">
+        <v>116821</v>
+      </c>
+      <c r="M453">
+        <v>114601</v>
+      </c>
+    </row>
+    <row r="454" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A454" t="str">
+        <f t="shared" si="16"/>
+        <v>114601_126022</v>
+      </c>
+      <c r="B454" t="str">
+        <f t="shared" si="15"/>
+        <v>41-30</v>
+      </c>
+      <c r="C454" t="s">
+        <v>230</v>
+      </c>
+      <c r="G454">
+        <v>41</v>
+      </c>
+      <c r="H454">
+        <v>30</v>
+      </c>
+      <c r="K454">
+        <v>114601</v>
+      </c>
+      <c r="M454">
+        <v>126022</v>
+      </c>
+    </row>
+    <row r="455" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A455" t="str">
+        <f t="shared" si="16"/>
+        <v>126022_123322</v>
+      </c>
+      <c r="B455" t="str">
+        <f t="shared" si="15"/>
+        <v>43-30</v>
+      </c>
+      <c r="C455" t="s">
+        <v>230</v>
+      </c>
+      <c r="G455">
+        <v>43</v>
+      </c>
+      <c r="H455">
+        <v>30</v>
+      </c>
+      <c r="K455">
+        <v>126022</v>
+      </c>
+      <c r="M455">
+        <v>123322</v>
+      </c>
+    </row>
+    <row r="456" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A456" t="str">
+        <f t="shared" si="16"/>
+        <v>123322_122522</v>
+      </c>
+      <c r="B456" t="str">
+        <f t="shared" si="15"/>
+        <v>46-30</v>
+      </c>
+      <c r="C456" t="s">
+        <v>230</v>
+      </c>
+      <c r="G456">
+        <v>46</v>
+      </c>
+      <c r="H456">
+        <v>30</v>
+      </c>
+      <c r="K456">
+        <v>123322</v>
+      </c>
+      <c r="M456">
+        <v>122522</v>
+      </c>
+    </row>
+    <row r="457" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A457" t="str">
+        <f t="shared" si="16"/>
+        <v>122522_113522</v>
+      </c>
+      <c r="B457" t="str">
+        <f t="shared" si="15"/>
+        <v>48-28</v>
+      </c>
+      <c r="C457" t="s">
+        <v>230</v>
+      </c>
+      <c r="G457">
+        <v>48</v>
+      </c>
+      <c r="H457">
+        <v>28</v>
+      </c>
+      <c r="K457">
+        <v>122522</v>
+      </c>
+      <c r="M457">
+        <v>113522</v>
+      </c>
+    </row>
+    <row r="458" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A458" t="str">
+        <f t="shared" si="16"/>
+        <v>113522_113602</v>
+      </c>
+      <c r="B458" t="str">
+        <f t="shared" si="15"/>
+        <v>51-25</v>
+      </c>
+      <c r="C458" t="s">
+        <v>230</v>
+      </c>
+      <c r="G458">
+        <v>51</v>
+      </c>
+      <c r="H458">
+        <v>25</v>
+      </c>
+      <c r="K458">
+        <v>113522</v>
+      </c>
+      <c r="M458">
+        <v>113602</v>
+      </c>
+    </row>
+    <row r="459" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A459" t="str">
+        <f t="shared" si="16"/>
+        <v>113602_113302</v>
+      </c>
+      <c r="B459" t="str">
+        <f t="shared" si="15"/>
+        <v>55-25</v>
+      </c>
+      <c r="C459" t="s">
+        <v>230</v>
+      </c>
+      <c r="D459" t="s">
+        <v>245</v>
+      </c>
+      <c r="G459">
+        <v>55</v>
+      </c>
+      <c r="H459">
+        <v>25</v>
+      </c>
+      <c r="K459">
+        <v>113602</v>
+      </c>
+      <c r="M459">
+        <v>113302</v>
+      </c>
+    </row>
+    <row r="460" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A460" t="str">
+        <f t="shared" si="16"/>
+        <v>113302_51602</v>
+      </c>
+      <c r="B460" t="str">
+        <f t="shared" si="15"/>
+        <v>57-25</v>
+      </c>
+      <c r="C460" t="s">
+        <v>230</v>
+      </c>
+      <c r="G460">
+        <v>57</v>
+      </c>
+      <c r="H460">
+        <v>25</v>
+      </c>
+      <c r="K460">
+        <v>113302</v>
+      </c>
+      <c r="M460">
+        <v>51602</v>
+      </c>
+    </row>
+    <row r="461" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A461" t="str">
+        <f t="shared" si="16"/>
+        <v>51602_51502</v>
+      </c>
+      <c r="B461" t="str">
+        <f t="shared" si="15"/>
+        <v>59-25</v>
+      </c>
+      <c r="C461" t="s">
+        <v>230</v>
+      </c>
+      <c r="G461">
+        <v>59</v>
+      </c>
+      <c r="H461">
+        <v>25</v>
+      </c>
+      <c r="K461">
+        <v>51602</v>
+      </c>
+      <c r="M461">
+        <v>51502</v>
+      </c>
+    </row>
+    <row r="462" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A462" t="str">
+        <f t="shared" si="16"/>
+        <v>51502_574202</v>
+      </c>
+      <c r="B462" t="str">
+        <f t="shared" si="15"/>
+        <v>61-25</v>
+      </c>
+      <c r="C462" t="s">
+        <v>230</v>
+      </c>
+      <c r="D462" t="s">
+        <v>237</v>
+      </c>
+      <c r="G462">
+        <v>61</v>
+      </c>
+      <c r="H462">
+        <v>25</v>
+      </c>
+      <c r="K462">
+        <v>51502</v>
+      </c>
+      <c r="M462">
+        <v>574202</v>
+      </c>
+    </row>
+    <row r="463" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A463" t="str">
+        <f t="shared" ref="A463:A520" si="17">_xlfn.CONCAT(K463,"_",L463,"_",M463)</f>
+        <v>574201_51501_51601</v>
+      </c>
+      <c r="B463" t="str">
+        <f t="shared" si="15"/>
+        <v>60-24</v>
+      </c>
+      <c r="C463" t="s">
+        <v>232</v>
+      </c>
+      <c r="D463" t="s">
+        <v>240</v>
+      </c>
+      <c r="G463">
+        <v>60</v>
+      </c>
+      <c r="H463">
+        <v>24</v>
+      </c>
+      <c r="K463">
+        <v>574201</v>
+      </c>
+      <c r="L463">
+        <v>51501</v>
+      </c>
+      <c r="M463">
+        <v>51601</v>
+      </c>
+    </row>
+    <row r="464" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A464" t="str">
+        <f t="shared" si="17"/>
+        <v>51501_51601_113301</v>
+      </c>
+      <c r="B464" t="str">
+        <f t="shared" si="15"/>
+        <v>58-24</v>
+      </c>
+      <c r="C464" t="s">
+        <v>232</v>
+      </c>
+      <c r="G464">
+        <v>58</v>
+      </c>
+      <c r="H464">
+        <v>24</v>
+      </c>
+      <c r="K464">
+        <v>51501</v>
+      </c>
+      <c r="L464">
+        <v>51601</v>
+      </c>
+      <c r="M464">
+        <v>113301</v>
+      </c>
+    </row>
+    <row r="465" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A465" t="str">
+        <f t="shared" si="17"/>
+        <v>51601_113301_113601</v>
+      </c>
+      <c r="B465" t="str">
+        <f t="shared" si="15"/>
+        <v>56-24</v>
+      </c>
+      <c r="C465" t="s">
+        <v>232</v>
+      </c>
+      <c r="D465" t="s">
+        <v>246</v>
+      </c>
+      <c r="G465">
+        <v>56</v>
+      </c>
+      <c r="H465">
+        <v>24</v>
+      </c>
+      <c r="K465">
+        <v>51601</v>
+      </c>
+      <c r="L465">
+        <v>113301</v>
+      </c>
+      <c r="M465">
+        <v>113601</v>
+      </c>
+    </row>
+    <row r="466" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A466" t="str">
+        <f t="shared" si="17"/>
+        <v>113301_113601_113521</v>
+      </c>
+      <c r="B466" t="str">
+        <f t="shared" si="15"/>
+        <v>52-24</v>
+      </c>
+      <c r="C466" t="s">
+        <v>232</v>
+      </c>
+      <c r="D466" t="s">
+        <v>247</v>
+      </c>
+      <c r="G466">
+        <v>52</v>
+      </c>
+      <c r="H466">
+        <v>24</v>
+      </c>
+      <c r="K466">
+        <v>113301</v>
+      </c>
+      <c r="L466">
+        <v>113601</v>
+      </c>
+      <c r="M466">
+        <v>113521</v>
+      </c>
+    </row>
+    <row r="467" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A467" t="str">
+        <f t="shared" si="17"/>
+        <v>113601_113521_122521</v>
+      </c>
+      <c r="B467" t="str">
+        <f t="shared" ref="B467:B522" si="18">_xlfn.CONCAT(G467,"-",H467)</f>
+        <v>48-26</v>
+      </c>
+      <c r="C467" t="s">
+        <v>232</v>
+      </c>
+      <c r="G467">
+        <v>48</v>
+      </c>
+      <c r="H467">
+        <v>26</v>
+      </c>
+      <c r="K467">
+        <v>113601</v>
+      </c>
+      <c r="L467">
+        <v>113521</v>
+      </c>
+      <c r="M467">
+        <v>122521</v>
+      </c>
+    </row>
+    <row r="468" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A468" t="str">
+        <f t="shared" si="17"/>
+        <v>113521_122521_123321</v>
+      </c>
+      <c r="B468" t="str">
+        <f t="shared" si="18"/>
+        <v>46-28</v>
+      </c>
+      <c r="C468" t="s">
+        <v>232</v>
+      </c>
+      <c r="G468">
+        <v>46</v>
+      </c>
+      <c r="H468">
+        <v>28</v>
+      </c>
+      <c r="K468">
+        <v>113521</v>
+      </c>
+      <c r="L468">
+        <v>122521</v>
+      </c>
+      <c r="M468">
+        <v>123321</v>
+      </c>
+    </row>
+    <row r="469" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A469" t="str">
+        <f t="shared" si="17"/>
+        <v>122521_123321_126021</v>
+      </c>
+      <c r="B469" t="str">
+        <f t="shared" si="18"/>
+        <v>44-29</v>
+      </c>
+      <c r="C469" t="s">
+        <v>232</v>
+      </c>
+      <c r="G469">
+        <v>44</v>
+      </c>
+      <c r="H469">
+        <v>29</v>
+      </c>
+      <c r="K469">
+        <v>122521</v>
+      </c>
+      <c r="L469">
+        <v>123321</v>
+      </c>
+      <c r="M469">
+        <v>126021</v>
+      </c>
+    </row>
+    <row r="470" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A470" t="str">
+        <f t="shared" si="17"/>
+        <v>123321_126021_114602</v>
+      </c>
+      <c r="B470" t="str">
+        <f t="shared" si="18"/>
+        <v>42-29</v>
+      </c>
+      <c r="C470" t="s">
+        <v>232</v>
+      </c>
+      <c r="G470">
+        <v>42</v>
+      </c>
+      <c r="H470">
+        <v>29</v>
+      </c>
+      <c r="K470">
+        <v>123321</v>
+      </c>
+      <c r="L470">
+        <v>126021</v>
+      </c>
+      <c r="M470">
+        <v>114602</v>
+      </c>
+    </row>
+    <row r="471" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A471" t="str">
+        <f t="shared" si="17"/>
+        <v>126021_114602_116822</v>
+      </c>
+      <c r="B471" t="str">
+        <f t="shared" si="18"/>
+        <v>40-29</v>
+      </c>
+      <c r="C471" t="s">
+        <v>232</v>
+      </c>
+      <c r="G471">
+        <v>40</v>
+      </c>
+      <c r="H471">
+        <v>29</v>
+      </c>
+      <c r="K471">
+        <v>126021</v>
+      </c>
+      <c r="L471">
+        <v>114602</v>
+      </c>
+      <c r="M471">
+        <v>116822</v>
+      </c>
+    </row>
+    <row r="472" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A472" t="str">
+        <f t="shared" si="17"/>
+        <v>114602_116822_119322</v>
+      </c>
+      <c r="B472" t="str">
+        <f t="shared" si="18"/>
+        <v>37-28</v>
+      </c>
+      <c r="C472" t="s">
+        <v>232</v>
+      </c>
+      <c r="G472">
+        <v>37</v>
+      </c>
+      <c r="H472">
+        <v>28</v>
+      </c>
+      <c r="K472">
+        <v>114602</v>
+      </c>
+      <c r="L472">
+        <v>116822</v>
+      </c>
+      <c r="M472">
+        <v>119322</v>
+      </c>
+    </row>
+    <row r="473" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A473" t="str">
+        <f t="shared" si="17"/>
+        <v>116822_119322_119402</v>
+      </c>
+      <c r="B473" t="str">
+        <f t="shared" si="18"/>
+        <v>37-26</v>
+      </c>
+      <c r="C473" t="s">
+        <v>232</v>
+      </c>
+      <c r="G473">
+        <v>37</v>
+      </c>
+      <c r="H473">
+        <v>26</v>
+      </c>
+      <c r="K473">
+        <v>116822</v>
+      </c>
+      <c r="L473">
+        <v>119322</v>
+      </c>
+      <c r="M473">
+        <v>119402</v>
+      </c>
+    </row>
+    <row r="474" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A474" t="str">
+        <f t="shared" si="17"/>
+        <v>119322_119402_116022</v>
+      </c>
+      <c r="B474" t="str">
+        <f t="shared" si="18"/>
+        <v>37-22</v>
+      </c>
+      <c r="C474" t="s">
+        <v>232</v>
+      </c>
+      <c r="G474">
+        <v>37</v>
+      </c>
+      <c r="H474">
+        <v>22</v>
+      </c>
+      <c r="K474">
+        <v>119322</v>
+      </c>
+      <c r="L474">
+        <v>119402</v>
+      </c>
+      <c r="M474">
+        <v>116022</v>
+      </c>
+    </row>
+    <row r="475" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A475" t="str">
+        <f t="shared" si="17"/>
+        <v>119402_116022_133002</v>
+      </c>
+      <c r="B475" t="str">
+        <f t="shared" si="18"/>
+        <v>37-20</v>
+      </c>
+      <c r="C475" t="s">
+        <v>232</v>
+      </c>
+      <c r="G475">
+        <v>37</v>
+      </c>
+      <c r="H475">
+        <v>20</v>
+      </c>
+      <c r="K475">
+        <v>119402</v>
+      </c>
+      <c r="L475">
+        <v>116022</v>
+      </c>
+      <c r="M475">
+        <v>133002</v>
+      </c>
+    </row>
+    <row r="476" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A476" t="str">
+        <f t="shared" si="17"/>
+        <v>116022_133002_133102</v>
+      </c>
+      <c r="B476" t="str">
+        <f t="shared" si="18"/>
+        <v>39-15</v>
+      </c>
+      <c r="C476" t="s">
+        <v>232</v>
+      </c>
+      <c r="G476">
+        <v>39</v>
+      </c>
+      <c r="H476">
+        <v>15</v>
+      </c>
+      <c r="K476">
+        <v>116022</v>
+      </c>
+      <c r="L476">
+        <v>133002</v>
+      </c>
+      <c r="M476">
+        <v>133102</v>
+      </c>
+    </row>
+    <row r="477" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A477" t="str">
+        <f t="shared" si="17"/>
+        <v>133002_133102_118002</v>
+      </c>
+      <c r="B477" t="str">
+        <f t="shared" si="18"/>
+        <v>41-13</v>
+      </c>
+      <c r="C477" t="s">
+        <v>232</v>
+      </c>
+      <c r="G477">
+        <v>41</v>
+      </c>
+      <c r="H477">
+        <v>13</v>
+      </c>
+      <c r="K477">
+        <v>133002</v>
+      </c>
+      <c r="L477">
+        <v>133102</v>
+      </c>
+      <c r="M477">
+        <v>118002</v>
+      </c>
+    </row>
+    <row r="478" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A478" t="str">
+        <f t="shared" si="17"/>
+        <v>133102_118002_169302</v>
+      </c>
+      <c r="B478" t="str">
+        <f t="shared" si="18"/>
+        <v>43-11</v>
+      </c>
+      <c r="C478" t="s">
+        <v>232</v>
+      </c>
+      <c r="G478">
+        <v>43</v>
+      </c>
+      <c r="H478">
+        <v>11</v>
+      </c>
+      <c r="K478">
+        <v>133102</v>
+      </c>
+      <c r="L478">
+        <v>118002</v>
+      </c>
+      <c r="M478">
+        <v>169302</v>
+      </c>
+    </row>
+    <row r="479" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A479" t="str">
+        <f t="shared" si="17"/>
+        <v>118002_169302_130202</v>
+      </c>
+      <c r="B479" t="str">
+        <f t="shared" si="18"/>
+        <v>45-9</v>
+      </c>
+      <c r="C479" t="s">
+        <v>232</v>
+      </c>
+      <c r="G479">
+        <v>45</v>
+      </c>
+      <c r="H479">
+        <v>9</v>
+      </c>
+      <c r="K479">
+        <v>118002</v>
+      </c>
+      <c r="L479">
+        <v>169302</v>
+      </c>
+      <c r="M479">
+        <v>130202</v>
+      </c>
+    </row>
+    <row r="480" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A480" t="str">
+        <f t="shared" si="17"/>
+        <v>169302_130202_130402</v>
+      </c>
+      <c r="B480" t="str">
+        <f t="shared" si="18"/>
+        <v>47-7</v>
+      </c>
+      <c r="C480" t="s">
+        <v>232</v>
+      </c>
+      <c r="G480">
+        <v>47</v>
+      </c>
+      <c r="H480">
+        <v>7</v>
+      </c>
+      <c r="K480">
+        <v>169302</v>
+      </c>
+      <c r="L480">
+        <v>130202</v>
+      </c>
+      <c r="M480">
+        <v>130402</v>
+      </c>
+    </row>
+    <row r="481" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A481" t="str">
+        <f t="shared" si="17"/>
+        <v>130202_130402_61901</v>
+      </c>
+      <c r="B481" t="str">
+        <f t="shared" si="18"/>
+        <v>49-5</v>
+      </c>
+      <c r="C481" t="s">
+        <v>232</v>
+      </c>
+      <c r="D481" t="s">
+        <v>241</v>
+      </c>
+      <c r="G481">
+        <v>49</v>
+      </c>
+      <c r="H481">
+        <v>5</v>
+      </c>
+      <c r="K481">
+        <v>130202</v>
+      </c>
+      <c r="L481">
+        <v>130402</v>
+      </c>
+      <c r="M481">
+        <v>61901</v>
+      </c>
+    </row>
+    <row r="482" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A482" t="str">
+        <f t="shared" si="17"/>
+        <v>61902_130401_130201</v>
+      </c>
+      <c r="B482" t="str">
+        <f t="shared" si="18"/>
+        <v>48-4</v>
+      </c>
+      <c r="C482" t="s">
+        <v>231</v>
+      </c>
+      <c r="D482" t="s">
+        <v>241</v>
+      </c>
+      <c r="G482">
+        <v>48</v>
+      </c>
+      <c r="H482">
+        <v>4</v>
+      </c>
+      <c r="K482">
+        <v>61902</v>
+      </c>
+      <c r="L482">
+        <v>130401</v>
+      </c>
+      <c r="M482">
+        <v>130201</v>
+      </c>
+    </row>
+    <row r="483" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A483" t="str">
+        <f t="shared" si="17"/>
+        <v>130401_130201_169301</v>
+      </c>
+      <c r="B483" t="str">
+        <f t="shared" si="18"/>
+        <v>46-6</v>
+      </c>
+      <c r="C483" t="s">
+        <v>231</v>
+      </c>
+      <c r="G483">
+        <v>46</v>
+      </c>
+      <c r="H483">
+        <v>6</v>
+      </c>
+      <c r="K483">
+        <v>130401</v>
+      </c>
+      <c r="L483">
+        <v>130201</v>
+      </c>
+      <c r="M483">
+        <v>169301</v>
+      </c>
+    </row>
+    <row r="484" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A484" t="str">
+        <f t="shared" si="17"/>
+        <v>130201_169301_118001</v>
+      </c>
+      <c r="B484" t="str">
+        <f t="shared" si="18"/>
+        <v>44-8</v>
+      </c>
+      <c r="C484" t="s">
+        <v>231</v>
+      </c>
+      <c r="G484">
+        <v>44</v>
+      </c>
+      <c r="H484">
+        <v>8</v>
+      </c>
+      <c r="K484">
+        <v>130201</v>
+      </c>
+      <c r="L484">
+        <v>169301</v>
+      </c>
+      <c r="M484">
+        <v>118001</v>
+      </c>
+    </row>
+    <row r="485" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A485" t="str">
+        <f t="shared" si="17"/>
+        <v>169301_118001_133101</v>
+      </c>
+      <c r="B485" t="str">
+        <f t="shared" si="18"/>
+        <v>42-10</v>
+      </c>
+      <c r="C485" t="s">
+        <v>231</v>
+      </c>
+      <c r="G485">
+        <v>42</v>
+      </c>
+      <c r="H485">
+        <v>10</v>
+      </c>
+      <c r="K485">
+        <v>169301</v>
+      </c>
+      <c r="L485">
+        <v>118001</v>
+      </c>
+      <c r="M485">
+        <v>133101</v>
+      </c>
+    </row>
+    <row r="486" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A486" t="str">
+        <f t="shared" si="17"/>
+        <v>118001_133101_133001</v>
+      </c>
+      <c r="B486" t="str">
+        <f t="shared" si="18"/>
+        <v>40-12</v>
+      </c>
+      <c r="C486" t="s">
+        <v>231</v>
+      </c>
+      <c r="G486">
+        <v>40</v>
+      </c>
+      <c r="H486">
+        <v>12</v>
+      </c>
+      <c r="K486">
+        <v>118001</v>
+      </c>
+      <c r="L486">
+        <v>133101</v>
+      </c>
+      <c r="M486">
+        <v>133001</v>
+      </c>
+    </row>
+    <row r="487" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A487" t="str">
+        <f t="shared" si="17"/>
+        <v>133101_133001_116021</v>
+      </c>
+      <c r="B487" t="str">
+        <f t="shared" si="18"/>
+        <v>38-14</v>
+      </c>
+      <c r="C487" t="s">
+        <v>231</v>
+      </c>
+      <c r="G487">
+        <v>38</v>
+      </c>
+      <c r="H487">
+        <v>14</v>
+      </c>
+      <c r="K487">
+        <v>133101</v>
+      </c>
+      <c r="L487">
+        <v>133001</v>
+      </c>
+      <c r="M487">
+        <v>116021</v>
+      </c>
+    </row>
+    <row r="488" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A488" t="str">
+        <f t="shared" si="17"/>
+        <v>133001_116021_119421</v>
+      </c>
+      <c r="B488" t="str">
+        <f t="shared" si="18"/>
+        <v>36-20</v>
+      </c>
+      <c r="C488" t="s">
+        <v>231</v>
+      </c>
+      <c r="G488">
+        <v>36</v>
+      </c>
+      <c r="H488">
+        <v>20</v>
+      </c>
+      <c r="K488">
+        <v>133001</v>
+      </c>
+      <c r="L488">
+        <v>116021</v>
+      </c>
+      <c r="M488">
+        <v>119421</v>
+      </c>
+    </row>
+    <row r="489" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A489" t="str">
+        <f t="shared" si="17"/>
+        <v>116021_119421_119321</v>
+      </c>
+      <c r="B489" t="str">
+        <f t="shared" si="18"/>
+        <v>36-22</v>
+      </c>
+      <c r="C489" t="s">
+        <v>231</v>
+      </c>
+      <c r="G489">
+        <v>36</v>
+      </c>
+      <c r="H489">
+        <v>22</v>
+      </c>
+      <c r="K489">
+        <v>116021</v>
+      </c>
+      <c r="L489">
+        <v>119421</v>
+      </c>
+      <c r="M489">
+        <v>119321</v>
+      </c>
+    </row>
+    <row r="490" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A490" t="str">
+        <f t="shared" si="17"/>
+        <v>119421_119321_116821</v>
+      </c>
+      <c r="B490" t="str">
+        <f t="shared" si="18"/>
+        <v>36-26</v>
+      </c>
+      <c r="C490" t="s">
+        <v>231</v>
+      </c>
+      <c r="G490">
+        <v>36</v>
+      </c>
+      <c r="H490">
+        <v>26</v>
+      </c>
+      <c r="K490">
+        <v>119421</v>
+      </c>
+      <c r="L490">
+        <v>119321</v>
+      </c>
+      <c r="M490">
+        <v>116821</v>
+      </c>
+    </row>
+    <row r="491" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A491" t="str">
+        <f t="shared" si="17"/>
+        <v>119321_116821_114601</v>
+      </c>
+      <c r="B491" t="str">
+        <f t="shared" si="18"/>
+        <v>36-28</v>
+      </c>
+      <c r="C491" t="s">
+        <v>231</v>
+      </c>
+      <c r="G491">
+        <v>36</v>
+      </c>
+      <c r="H491">
+        <v>28</v>
+      </c>
+      <c r="K491">
+        <v>119321</v>
+      </c>
+      <c r="L491">
+        <v>116821</v>
+      </c>
+      <c r="M491">
+        <v>114601</v>
+      </c>
+    </row>
+    <row r="492" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A492" t="str">
+        <f t="shared" si="17"/>
+        <v>116821_114601_126022</v>
+      </c>
+      <c r="B492" t="str">
+        <f t="shared" si="18"/>
+        <v>40-30</v>
+      </c>
+      <c r="C492" t="s">
+        <v>231</v>
+      </c>
+      <c r="G492">
+        <v>40</v>
+      </c>
+      <c r="H492">
+        <v>30</v>
+      </c>
+      <c r="K492">
+        <v>116821</v>
+      </c>
+      <c r="L492">
+        <v>114601</v>
+      </c>
+      <c r="M492">
+        <v>126022</v>
+      </c>
+    </row>
+    <row r="493" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A493" t="str">
+        <f t="shared" si="17"/>
+        <v>114601_126022_123322</v>
+      </c>
+      <c r="B493" t="str">
+        <f t="shared" si="18"/>
+        <v>42-30</v>
+      </c>
+      <c r="C493" t="s">
+        <v>231</v>
+      </c>
+      <c r="G493">
+        <v>42</v>
+      </c>
+      <c r="H493">
+        <v>30</v>
+      </c>
+      <c r="K493">
+        <v>114601</v>
+      </c>
+      <c r="L493">
+        <v>126022</v>
+      </c>
+      <c r="M493">
+        <v>123322</v>
+      </c>
+    </row>
+    <row r="494" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A494" t="str">
+        <f t="shared" si="17"/>
+        <v>126022_123322_122522</v>
+      </c>
+      <c r="B494" t="str">
+        <f t="shared" si="18"/>
+        <v>44-30</v>
+      </c>
+      <c r="C494" t="s">
+        <v>231</v>
+      </c>
+      <c r="G494">
+        <v>44</v>
+      </c>
+      <c r="H494">
+        <v>30</v>
+      </c>
+      <c r="K494">
+        <v>126022</v>
+      </c>
+      <c r="L494">
+        <v>123322</v>
+      </c>
+      <c r="M494">
+        <v>122522</v>
+      </c>
+    </row>
+    <row r="495" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A495" t="str">
+        <f t="shared" si="17"/>
+        <v>123322_122522_113522</v>
+      </c>
+      <c r="B495" t="str">
+        <f t="shared" si="18"/>
+        <v>47-29</v>
+      </c>
+      <c r="C495" t="s">
+        <v>231</v>
+      </c>
+      <c r="G495">
+        <v>47</v>
+      </c>
+      <c r="H495">
+        <v>29</v>
+      </c>
+      <c r="K495">
+        <v>123322</v>
+      </c>
+      <c r="L495">
+        <v>122522</v>
+      </c>
+      <c r="M495">
+        <v>113522</v>
+      </c>
+    </row>
+    <row r="496" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A496" t="str">
+        <f t="shared" si="17"/>
+        <v>122522_113522_113602</v>
+      </c>
+      <c r="B496" t="str">
+        <f t="shared" si="18"/>
+        <v>49-27</v>
+      </c>
+      <c r="C496" t="s">
+        <v>231</v>
+      </c>
+      <c r="G496">
+        <v>49</v>
+      </c>
+      <c r="H496">
+        <v>27</v>
+      </c>
+      <c r="K496">
+        <v>122522</v>
+      </c>
+      <c r="L496">
+        <v>113522</v>
+      </c>
+      <c r="M496">
+        <v>113602</v>
+      </c>
+    </row>
+    <row r="497" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A497" t="str">
+        <f t="shared" si="17"/>
+        <v>113522_113602_113302</v>
+      </c>
+      <c r="B497" t="str">
+        <f t="shared" si="18"/>
+        <v>52-25</v>
+      </c>
+      <c r="C497" t="s">
+        <v>231</v>
+      </c>
+      <c r="D497" t="s">
+        <v>248</v>
+      </c>
+      <c r="G497">
+        <v>52</v>
+      </c>
+      <c r="H497">
+        <v>25</v>
+      </c>
+      <c r="K497">
+        <v>113522</v>
+      </c>
+      <c r="L497">
+        <v>113602</v>
+      </c>
+      <c r="M497">
+        <v>113302</v>
+      </c>
+    </row>
+    <row r="498" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A498" t="str">
+        <f t="shared" si="17"/>
+        <v>113602_113302_51602</v>
+      </c>
+      <c r="B498" t="str">
+        <f t="shared" si="18"/>
+        <v>56-25</v>
+      </c>
+      <c r="C498" t="s">
+        <v>231</v>
+      </c>
+      <c r="D498" t="s">
+        <v>249</v>
+      </c>
+      <c r="G498">
+        <v>56</v>
+      </c>
+      <c r="H498">
+        <v>25</v>
+      </c>
+      <c r="K498">
+        <v>113602</v>
+      </c>
+      <c r="L498">
+        <v>113302</v>
+      </c>
+      <c r="M498">
+        <v>51602</v>
+      </c>
+    </row>
+    <row r="499" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A499" t="str">
+        <f t="shared" si="17"/>
+        <v>113302_51602_51502</v>
+      </c>
+      <c r="B499" t="str">
+        <f t="shared" si="18"/>
+        <v>58-25</v>
+      </c>
+      <c r="C499" t="s">
+        <v>231</v>
+      </c>
+      <c r="G499">
+        <v>58</v>
+      </c>
+      <c r="H499">
+        <v>25</v>
+      </c>
+      <c r="K499">
+        <v>113302</v>
+      </c>
+      <c r="L499">
+        <v>51602</v>
+      </c>
+      <c r="M499">
+        <v>51502</v>
+      </c>
+    </row>
+    <row r="500" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A500" t="str">
+        <f t="shared" si="17"/>
+        <v>51602_51502_574202</v>
+      </c>
+      <c r="B500" t="str">
+        <f t="shared" si="18"/>
+        <v>60-25</v>
+      </c>
+      <c r="C500" t="s">
+        <v>231</v>
+      </c>
+      <c r="D500" t="s">
+        <v>240</v>
+      </c>
+      <c r="G500">
+        <v>60</v>
+      </c>
+      <c r="H500">
+        <v>25</v>
+      </c>
+      <c r="K500">
+        <v>51602</v>
+      </c>
+      <c r="L500">
+        <v>51502</v>
+      </c>
+      <c r="M500">
+        <v>574202</v>
+      </c>
+    </row>
+    <row r="501" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A501" t="str">
+        <f t="shared" si="17"/>
+        <v>574201_51501_DEPOT</v>
+      </c>
+      <c r="B501" t="str">
+        <f t="shared" si="18"/>
+        <v>60-24</v>
+      </c>
+      <c r="C501" t="s">
+        <v>233</v>
+      </c>
+      <c r="D501" t="s">
+        <v>240</v>
+      </c>
+      <c r="G501">
+        <v>60</v>
+      </c>
+      <c r="H501">
+        <v>24</v>
+      </c>
+      <c r="K501">
+        <v>574201</v>
+      </c>
+      <c r="L501">
+        <v>51501</v>
+      </c>
+      <c r="M501" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="502" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A502" t="str">
+        <f t="shared" si="17"/>
+        <v>51501_51601_DEPOT</v>
+      </c>
+      <c r="B502" t="str">
+        <f t="shared" si="18"/>
+        <v>58-24</v>
+      </c>
+      <c r="C502" t="s">
+        <v>233</v>
+      </c>
+      <c r="G502">
+        <v>58</v>
+      </c>
+      <c r="H502">
+        <v>24</v>
+      </c>
+      <c r="K502">
+        <v>51501</v>
+      </c>
+      <c r="L502">
+        <v>51601</v>
+      </c>
+      <c r="M502" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="503" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A503" t="str">
+        <f t="shared" si="17"/>
+        <v>51601_113301_DEPOT</v>
+      </c>
+      <c r="B503" t="str">
+        <f t="shared" si="18"/>
+        <v>56-24</v>
+      </c>
+      <c r="C503" t="s">
+        <v>233</v>
+      </c>
+      <c r="G503">
+        <v>56</v>
+      </c>
+      <c r="H503">
+        <v>24</v>
+      </c>
+      <c r="K503">
+        <v>51601</v>
+      </c>
+      <c r="L503">
+        <v>113301</v>
+      </c>
+      <c r="M503" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="504" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A504" t="str">
+        <f t="shared" si="17"/>
+        <v>113301_113601_DEPOT</v>
+      </c>
+      <c r="B504" t="str">
+        <f t="shared" si="18"/>
+        <v>52-24</v>
+      </c>
+      <c r="C504" t="s">
+        <v>233</v>
+      </c>
+      <c r="G504">
+        <v>52</v>
+      </c>
+      <c r="H504">
+        <v>24</v>
+      </c>
+      <c r="K504">
+        <v>113301</v>
+      </c>
+      <c r="L504">
+        <v>113601</v>
+      </c>
+      <c r="M504" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="505" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A505" t="str">
+        <f t="shared" si="17"/>
+        <v>113601_113521_DEPOT</v>
+      </c>
+      <c r="B505" t="str">
+        <f t="shared" si="18"/>
+        <v>48-26</v>
+      </c>
+      <c r="C505" t="s">
+        <v>233</v>
+      </c>
+      <c r="G505">
+        <v>48</v>
+      </c>
+      <c r="H505">
+        <v>26</v>
+      </c>
+      <c r="K505">
+        <v>113601</v>
+      </c>
+      <c r="L505">
+        <v>113521</v>
+      </c>
+      <c r="M505" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="506" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A506" t="str">
+        <f t="shared" si="17"/>
+        <v>113521_122521_DEPOT</v>
+      </c>
+      <c r="B506" t="str">
+        <f t="shared" si="18"/>
+        <v>46-28</v>
+      </c>
+      <c r="C506" t="s">
+        <v>233</v>
+      </c>
+      <c r="G506">
+        <v>46</v>
+      </c>
+      <c r="H506">
+        <v>28</v>
+      </c>
+      <c r="K506">
+        <v>113521</v>
+      </c>
+      <c r="L506">
+        <v>122521</v>
+      </c>
+      <c r="M506" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="507" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A507" t="str">
+        <f t="shared" si="17"/>
+        <v>122521_123321_DEPOT</v>
+      </c>
+      <c r="B507" t="str">
+        <f t="shared" si="18"/>
+        <v>44-29</v>
+      </c>
+      <c r="C507" t="s">
+        <v>233</v>
+      </c>
+      <c r="G507">
+        <v>44</v>
+      </c>
+      <c r="H507">
+        <v>29</v>
+      </c>
+      <c r="K507">
+        <v>122521</v>
+      </c>
+      <c r="L507">
+        <v>123321</v>
+      </c>
+      <c r="M507" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="508" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A508" t="str">
+        <f t="shared" si="17"/>
+        <v>123321_126021_DEPOT</v>
+      </c>
+      <c r="B508" t="str">
+        <f t="shared" si="18"/>
+        <v>42-29</v>
+      </c>
+      <c r="C508" t="s">
+        <v>233</v>
+      </c>
+      <c r="G508">
+        <v>42</v>
+      </c>
+      <c r="H508">
+        <v>29</v>
+      </c>
+      <c r="K508">
+        <v>123321</v>
+      </c>
+      <c r="L508">
+        <v>126021</v>
+      </c>
+      <c r="M508" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="509" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A509" t="str">
+        <f t="shared" si="17"/>
+        <v>126021_114602_DEPOT</v>
+      </c>
+      <c r="B509" t="str">
+        <f t="shared" si="18"/>
+        <v>40-29</v>
+      </c>
+      <c r="C509" t="s">
+        <v>233</v>
+      </c>
+      <c r="G509">
+        <v>40</v>
+      </c>
+      <c r="H509">
+        <v>29</v>
+      </c>
+      <c r="K509">
+        <v>126021</v>
+      </c>
+      <c r="L509">
+        <v>114602</v>
+      </c>
+      <c r="M509" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="510" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A510" t="str">
+        <f t="shared" si="17"/>
+        <v>114602_116822_DEPOT</v>
+      </c>
+      <c r="B510" t="str">
+        <f t="shared" si="18"/>
+        <v>37-28</v>
+      </c>
+      <c r="C510" t="s">
+        <v>233</v>
+      </c>
+      <c r="G510">
+        <v>37</v>
+      </c>
+      <c r="H510">
+        <v>28</v>
+      </c>
+      <c r="K510">
+        <v>114602</v>
+      </c>
+      <c r="L510">
+        <v>116822</v>
+      </c>
+      <c r="M510" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="511" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A511" t="str">
+        <f t="shared" si="17"/>
+        <v>116822_119322_DEPOT</v>
+      </c>
+      <c r="B511" t="str">
+        <f t="shared" si="18"/>
+        <v>37-26</v>
+      </c>
+      <c r="C511" t="s">
+        <v>233</v>
+      </c>
+      <c r="G511">
+        <v>37</v>
+      </c>
+      <c r="H511">
+        <v>26</v>
+      </c>
+      <c r="K511">
+        <v>116822</v>
+      </c>
+      <c r="L511">
+        <v>119322</v>
+      </c>
+      <c r="M511" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="512" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A512" t="str">
+        <f t="shared" si="17"/>
+        <v>119322_119402_DEPOT</v>
+      </c>
+      <c r="B512" t="str">
+        <f t="shared" si="18"/>
+        <v>37-22</v>
+      </c>
+      <c r="C512" t="s">
+        <v>233</v>
+      </c>
+      <c r="G512">
+        <v>37</v>
+      </c>
+      <c r="H512">
+        <v>22</v>
+      </c>
+      <c r="K512">
+        <v>119322</v>
+      </c>
+      <c r="L512">
+        <v>119402</v>
+      </c>
+      <c r="M512" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="513" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A513" t="str">
+        <f t="shared" si="17"/>
+        <v>119402_116022_DEPOT</v>
+      </c>
+      <c r="B513" t="str">
+        <f t="shared" si="18"/>
+        <v>37-20</v>
+      </c>
+      <c r="C513" t="s">
+        <v>233</v>
+      </c>
+      <c r="G513">
+        <v>37</v>
+      </c>
+      <c r="H513">
+        <v>20</v>
+      </c>
+      <c r="K513">
+        <v>119402</v>
+      </c>
+      <c r="L513">
+        <v>116022</v>
+      </c>
+      <c r="M513" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="514" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A514" t="str">
+        <f t="shared" si="17"/>
+        <v>116022_133002_DEPOT</v>
+      </c>
+      <c r="B514" t="str">
+        <f t="shared" si="18"/>
+        <v>39-15</v>
+      </c>
+      <c r="C514" t="s">
+        <v>233</v>
+      </c>
+      <c r="G514">
+        <v>39</v>
+      </c>
+      <c r="H514">
+        <v>15</v>
+      </c>
+      <c r="K514">
+        <v>116022</v>
+      </c>
+      <c r="L514">
+        <v>133002</v>
+      </c>
+      <c r="M514" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="515" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A515" t="str">
+        <f t="shared" si="17"/>
+        <v>133002_133102_DEPOT</v>
+      </c>
+      <c r="B515" t="str">
+        <f t="shared" si="18"/>
+        <v>41-13</v>
+      </c>
+      <c r="C515" t="s">
+        <v>233</v>
+      </c>
+      <c r="G515">
+        <v>41</v>
+      </c>
+      <c r="H515">
+        <v>13</v>
+      </c>
+      <c r="K515">
+        <v>133002</v>
+      </c>
+      <c r="L515">
+        <v>133102</v>
+      </c>
+      <c r="M515" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="516" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A516" t="str">
+        <f t="shared" si="17"/>
+        <v>133102_118002_DEPOT</v>
+      </c>
+      <c r="B516" t="str">
+        <f t="shared" si="18"/>
+        <v>43-11</v>
+      </c>
+      <c r="C516" t="s">
+        <v>233</v>
+      </c>
+      <c r="G516">
+        <v>43</v>
+      </c>
+      <c r="H516">
+        <v>11</v>
+      </c>
+      <c r="K516">
+        <v>133102</v>
+      </c>
+      <c r="L516">
+        <v>118002</v>
+      </c>
+      <c r="M516" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="517" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A517" t="str">
+        <f t="shared" si="17"/>
+        <v>118002_169302_DEPOT</v>
+      </c>
+      <c r="B517" t="str">
+        <f t="shared" si="18"/>
+        <v>45-9</v>
+      </c>
+      <c r="C517" t="s">
+        <v>233</v>
+      </c>
+      <c r="G517">
+        <v>45</v>
+      </c>
+      <c r="H517">
+        <v>9</v>
+      </c>
+      <c r="K517">
+        <v>118002</v>
+      </c>
+      <c r="L517">
+        <v>169302</v>
+      </c>
+      <c r="M517" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="518" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A518" t="str">
+        <f t="shared" si="17"/>
+        <v>169302_130202_DEPOT</v>
+      </c>
+      <c r="B518" t="str">
+        <f t="shared" si="18"/>
+        <v>47-7</v>
+      </c>
+      <c r="C518" t="s">
+        <v>233</v>
+      </c>
+      <c r="G518">
+        <v>47</v>
+      </c>
+      <c r="H518">
+        <v>7</v>
+      </c>
+      <c r="K518">
+        <v>169302</v>
+      </c>
+      <c r="L518">
+        <v>130202</v>
+      </c>
+      <c r="M518" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="519" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A519" t="str">
+        <f t="shared" si="17"/>
+        <v>130202_130402_DEPOT</v>
+      </c>
+      <c r="B519" t="str">
+        <f t="shared" si="18"/>
+        <v>49-5</v>
+      </c>
+      <c r="C519" t="s">
+        <v>233</v>
+      </c>
+      <c r="G519">
+        <v>49</v>
+      </c>
+      <c r="H519">
+        <v>5</v>
+      </c>
+      <c r="K519">
+        <v>130202</v>
+      </c>
+      <c r="L519">
+        <v>130402</v>
+      </c>
+      <c r="M519" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="520" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A520" t="str">
+        <f t="shared" si="17"/>
+        <v>130402_61901_DEPOT</v>
+      </c>
+      <c r="B520" t="str">
+        <f t="shared" si="18"/>
+        <v>50-2</v>
+      </c>
+      <c r="C520" t="s">
+        <v>233</v>
+      </c>
+      <c r="D520" t="s">
+        <v>242</v>
+      </c>
+      <c r="G520">
+        <v>50</v>
+      </c>
+      <c r="H520">
+        <v>2</v>
+      </c>
+      <c r="K520">
+        <v>130402</v>
+      </c>
+      <c r="L520">
+        <v>61901</v>
+      </c>
+      <c r="M520" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="521" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A521" t="str">
+        <f t="shared" ref="A521:A578" si="19">_xlfn.CONCAT(K521,"_",L521,"_",M521)</f>
+        <v>61902_130401_DEPOT</v>
+      </c>
+      <c r="B521" t="str">
+        <f t="shared" si="18"/>
+        <v>48-4</v>
+      </c>
+      <c r="C521" t="s">
+        <v>234</v>
+      </c>
+      <c r="D521" t="s">
+        <v>241</v>
+      </c>
+      <c r="G521">
+        <v>48</v>
+      </c>
+      <c r="H521">
+        <v>4</v>
+      </c>
+      <c r="K521">
+        <v>61902</v>
+      </c>
+      <c r="L521">
+        <v>130401</v>
+      </c>
+      <c r="M521" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="522" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A522" t="str">
+        <f t="shared" si="19"/>
+        <v>130401_130201_DEPOT</v>
+      </c>
+      <c r="B522" t="str">
+        <f t="shared" si="18"/>
+        <v>46-6</v>
+      </c>
+      <c r="C522" t="s">
+        <v>234</v>
+      </c>
+      <c r="G522">
+        <v>46</v>
+      </c>
+      <c r="H522">
+        <v>6</v>
+      </c>
+      <c r="K522">
+        <v>130401</v>
+      </c>
+      <c r="L522">
+        <v>130201</v>
+      </c>
+      <c r="M522" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="523" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A523" t="str">
+        <f t="shared" si="19"/>
+        <v>130201_169301_DEPOT</v>
+      </c>
+      <c r="B523" t="str">
+        <f t="shared" ref="B523:B580" si="20">_xlfn.CONCAT(G523,"-",H523)</f>
+        <v>44-8</v>
+      </c>
+      <c r="C523" t="s">
+        <v>234</v>
+      </c>
+      <c r="G523">
+        <v>44</v>
+      </c>
+      <c r="H523">
+        <v>8</v>
+      </c>
+      <c r="K523">
+        <v>130201</v>
+      </c>
+      <c r="L523">
+        <v>169301</v>
+      </c>
+      <c r="M523" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="524" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A524" t="str">
+        <f t="shared" si="19"/>
+        <v>169301_118001_DEPOT</v>
+      </c>
+      <c r="B524" t="str">
+        <f t="shared" si="20"/>
+        <v>42-10</v>
+      </c>
+      <c r="C524" t="s">
+        <v>234</v>
+      </c>
+      <c r="G524">
+        <v>42</v>
+      </c>
+      <c r="H524">
+        <v>10</v>
+      </c>
+      <c r="K524">
+        <v>169301</v>
+      </c>
+      <c r="L524">
+        <v>118001</v>
+      </c>
+      <c r="M524" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="525" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A525" t="str">
+        <f t="shared" si="19"/>
+        <v>118001_133101_DEPOT</v>
+      </c>
+      <c r="B525" t="str">
+        <f t="shared" si="20"/>
+        <v>40-12</v>
+      </c>
+      <c r="C525" t="s">
+        <v>234</v>
+      </c>
+      <c r="G525">
+        <v>40</v>
+      </c>
+      <c r="H525">
+        <v>12</v>
+      </c>
+      <c r="K525">
+        <v>118001</v>
+      </c>
+      <c r="L525">
+        <v>133101</v>
+      </c>
+      <c r="M525" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="526" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A526" t="str">
+        <f t="shared" si="19"/>
+        <v>133101_133001_DEPOT</v>
+      </c>
+      <c r="B526" t="str">
+        <f t="shared" si="20"/>
+        <v>38-14</v>
+      </c>
+      <c r="C526" t="s">
+        <v>234</v>
+      </c>
+      <c r="G526">
+        <v>38</v>
+      </c>
+      <c r="H526">
+        <v>14</v>
+      </c>
+      <c r="K526">
+        <v>133101</v>
+      </c>
+      <c r="L526">
+        <v>133001</v>
+      </c>
+      <c r="M526" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="527" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A527" t="str">
+        <f t="shared" si="19"/>
+        <v>133001_116021_DEPOT</v>
+      </c>
+      <c r="B527" t="str">
+        <f t="shared" si="20"/>
+        <v>36-20</v>
+      </c>
+      <c r="C527" t="s">
+        <v>234</v>
+      </c>
+      <c r="G527">
+        <v>36</v>
+      </c>
+      <c r="H527">
+        <v>20</v>
+      </c>
+      <c r="K527">
+        <v>133001</v>
+      </c>
+      <c r="L527">
+        <v>116021</v>
+      </c>
+      <c r="M527" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="528" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A528" t="str">
+        <f t="shared" si="19"/>
+        <v>116021_119421_DEPOT</v>
+      </c>
+      <c r="B528" t="str">
+        <f t="shared" si="20"/>
+        <v>36-22</v>
+      </c>
+      <c r="C528" t="s">
+        <v>234</v>
+      </c>
+      <c r="G528">
+        <v>36</v>
+      </c>
+      <c r="H528">
+        <v>22</v>
+      </c>
+      <c r="K528">
+        <v>116021</v>
+      </c>
+      <c r="L528">
+        <v>119421</v>
+      </c>
+      <c r="M528" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="529" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A529" t="str">
+        <f t="shared" si="19"/>
+        <v>119421_119321_DEPOT</v>
+      </c>
+      <c r="B529" t="str">
+        <f t="shared" si="20"/>
+        <v>36-26</v>
+      </c>
+      <c r="C529" t="s">
+        <v>234</v>
+      </c>
+      <c r="G529">
+        <v>36</v>
+      </c>
+      <c r="H529">
+        <v>26</v>
+      </c>
+      <c r="K529">
+        <v>119421</v>
+      </c>
+      <c r="L529">
+        <v>119321</v>
+      </c>
+      <c r="M529" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="530" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A530" t="str">
+        <f t="shared" si="19"/>
+        <v>119321_116821_DEPOT</v>
+      </c>
+      <c r="B530" t="str">
+        <f t="shared" si="20"/>
+        <v>36-28</v>
+      </c>
+      <c r="C530" t="s">
+        <v>234</v>
+      </c>
+      <c r="G530">
+        <v>36</v>
+      </c>
+      <c r="H530">
+        <v>28</v>
+      </c>
+      <c r="K530">
+        <v>119321</v>
+      </c>
+      <c r="L530">
+        <v>116821</v>
+      </c>
+      <c r="M530" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="531" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A531" t="str">
+        <f t="shared" si="19"/>
+        <v>116821_114601_DEPOT</v>
+      </c>
+      <c r="B531" t="str">
+        <f t="shared" si="20"/>
+        <v>40-30</v>
+      </c>
+      <c r="C531" t="s">
+        <v>234</v>
+      </c>
+      <c r="G531">
+        <v>40</v>
+      </c>
+      <c r="H531">
+        <v>30</v>
+      </c>
+      <c r="K531">
+        <v>116821</v>
+      </c>
+      <c r="L531">
+        <v>114601</v>
+      </c>
+      <c r="M531" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="532" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A532" t="str">
+        <f t="shared" si="19"/>
+        <v>114601_126022_DEPOT</v>
+      </c>
+      <c r="B532" t="str">
+        <f t="shared" si="20"/>
+        <v>42-30</v>
+      </c>
+      <c r="C532" t="s">
+        <v>234</v>
+      </c>
+      <c r="G532">
+        <v>42</v>
+      </c>
+      <c r="H532">
+        <v>30</v>
+      </c>
+      <c r="K532">
+        <v>114601</v>
+      </c>
+      <c r="L532">
+        <v>126022</v>
+      </c>
+      <c r="M532" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="533" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A533" t="str">
+        <f t="shared" si="19"/>
+        <v>126022_123322_DEPOT</v>
+      </c>
+      <c r="B533" t="str">
+        <f t="shared" si="20"/>
+        <v>44-30</v>
+      </c>
+      <c r="C533" t="s">
+        <v>234</v>
+      </c>
+      <c r="G533">
+        <v>44</v>
+      </c>
+      <c r="H533">
+        <v>30</v>
+      </c>
+      <c r="K533">
+        <v>126022</v>
+      </c>
+      <c r="L533">
+        <v>123322</v>
+      </c>
+      <c r="M533" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="534" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A534" t="str">
+        <f t="shared" si="19"/>
+        <v>123322_122522_DEPOT</v>
+      </c>
+      <c r="B534" t="str">
+        <f t="shared" si="20"/>
+        <v>47-29</v>
+      </c>
+      <c r="C534" t="s">
+        <v>234</v>
+      </c>
+      <c r="G534">
+        <v>47</v>
+      </c>
+      <c r="H534">
+        <v>29</v>
+      </c>
+      <c r="K534">
+        <v>123322</v>
+      </c>
+      <c r="L534">
+        <v>122522</v>
+      </c>
+      <c r="M534" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="535" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A535" t="str">
+        <f t="shared" si="19"/>
+        <v>122522_113522_DEPOT</v>
+      </c>
+      <c r="B535" t="str">
+        <f t="shared" si="20"/>
+        <v>49-27</v>
+      </c>
+      <c r="C535" t="s">
+        <v>234</v>
+      </c>
+      <c r="G535">
+        <v>49</v>
+      </c>
+      <c r="H535">
+        <v>27</v>
+      </c>
+      <c r="K535">
+        <v>122522</v>
+      </c>
+      <c r="L535">
+        <v>113522</v>
+      </c>
+      <c r="M535" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="536" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A536" t="str">
+        <f t="shared" si="19"/>
+        <v>113522_113602_DEPOT</v>
+      </c>
+      <c r="B536" t="str">
+        <f t="shared" si="20"/>
+        <v>52-25</v>
+      </c>
+      <c r="C536" t="s">
+        <v>234</v>
+      </c>
+      <c r="G536">
+        <v>52</v>
+      </c>
+      <c r="H536">
+        <v>25</v>
+      </c>
+      <c r="K536">
+        <v>113522</v>
+      </c>
+      <c r="L536">
+        <v>113602</v>
+      </c>
+      <c r="M536" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="537" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A537" t="str">
+        <f t="shared" si="19"/>
+        <v>113602_113302_DEPOT</v>
+      </c>
+      <c r="B537" t="str">
+        <f t="shared" si="20"/>
+        <v>56-25</v>
+      </c>
+      <c r="C537" t="s">
+        <v>234</v>
+      </c>
+      <c r="G537">
+        <v>56</v>
+      </c>
+      <c r="H537">
+        <v>25</v>
+      </c>
+      <c r="K537">
+        <v>113602</v>
+      </c>
+      <c r="L537">
+        <v>113302</v>
+      </c>
+      <c r="M537" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="538" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A538" t="str">
+        <f t="shared" si="19"/>
+        <v>113302_51602_DEPOT</v>
+      </c>
+      <c r="B538" t="str">
+        <f t="shared" si="20"/>
+        <v>58-25</v>
+      </c>
+      <c r="C538" t="s">
+        <v>234</v>
+      </c>
+      <c r="G538">
+        <v>58</v>
+      </c>
+      <c r="H538">
+        <v>25</v>
+      </c>
+      <c r="K538">
+        <v>113302</v>
+      </c>
+      <c r="L538">
+        <v>51602</v>
+      </c>
+      <c r="M538" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="539" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A539" t="str">
+        <f t="shared" si="19"/>
+        <v>51602_51502_DEPOT</v>
+      </c>
+      <c r="B539" t="str">
+        <f t="shared" si="20"/>
+        <v>60-25</v>
+      </c>
+      <c r="C539" t="s">
+        <v>234</v>
+      </c>
+      <c r="G539">
+        <v>60</v>
+      </c>
+      <c r="H539">
+        <v>25</v>
+      </c>
+      <c r="K539">
+        <v>51602</v>
+      </c>
+      <c r="L539">
+        <v>51502</v>
+      </c>
+      <c r="M539" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="540" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A540" t="str">
+        <f t="shared" si="19"/>
+        <v>51502_574202_DEPOT</v>
+      </c>
+      <c r="B540" t="str">
+        <f t="shared" si="20"/>
+        <v>62-25</v>
+      </c>
+      <c r="C540" t="s">
+        <v>234</v>
+      </c>
+      <c r="D540" t="s">
+        <v>243</v>
+      </c>
+      <c r="G540">
+        <v>62</v>
+      </c>
+      <c r="H540">
+        <v>25</v>
+      </c>
+      <c r="K540">
+        <v>51502</v>
+      </c>
+      <c r="L540">
+        <v>574202</v>
+      </c>
+      <c r="M540" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="541" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A541" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_574201_51501</v>
+      </c>
+      <c r="B541" t="str">
+        <f t="shared" si="20"/>
+        <v>62-24</v>
+      </c>
+      <c r="C541" t="s">
+        <v>235</v>
+      </c>
+      <c r="D541" t="s">
+        <v>243</v>
+      </c>
+      <c r="G541">
+        <v>62</v>
+      </c>
+      <c r="H541">
+        <v>24</v>
+      </c>
+      <c r="K541" t="s">
+        <v>121</v>
+      </c>
+      <c r="L541">
+        <v>574201</v>
+      </c>
+      <c r="M541">
+        <v>51501</v>
+      </c>
+    </row>
+    <row r="542" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A542" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_51501_51601</v>
+      </c>
+      <c r="B542" t="str">
+        <f t="shared" si="20"/>
+        <v>60-24</v>
+      </c>
+      <c r="C542" t="s">
+        <v>235</v>
+      </c>
+      <c r="G542">
+        <v>60</v>
+      </c>
+      <c r="H542">
+        <v>24</v>
+      </c>
+      <c r="K542" t="s">
+        <v>121</v>
+      </c>
+      <c r="L542">
+        <v>51501</v>
+      </c>
+      <c r="M542">
+        <v>51601</v>
+      </c>
+    </row>
+    <row r="543" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A543" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_51601_113301</v>
+      </c>
+      <c r="B543" t="str">
+        <f t="shared" si="20"/>
+        <v>58-24</v>
+      </c>
+      <c r="C543" t="s">
+        <v>235</v>
+      </c>
+      <c r="G543">
+        <v>58</v>
+      </c>
+      <c r="H543">
+        <v>24</v>
+      </c>
+      <c r="K543" t="s">
+        <v>121</v>
+      </c>
+      <c r="L543">
+        <v>51601</v>
+      </c>
+      <c r="M543">
+        <v>113301</v>
+      </c>
+    </row>
+    <row r="544" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A544" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_113301_113601</v>
+      </c>
+      <c r="B544" t="str">
+        <f t="shared" si="20"/>
+        <v>56-24</v>
+      </c>
+      <c r="C544" t="s">
+        <v>235</v>
+      </c>
+      <c r="G544">
+        <v>56</v>
+      </c>
+      <c r="H544">
+        <v>24</v>
+      </c>
+      <c r="K544" t="s">
+        <v>121</v>
+      </c>
+      <c r="L544">
+        <v>113301</v>
+      </c>
+      <c r="M544">
+        <v>113601</v>
+      </c>
+    </row>
+    <row r="545" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A545" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_113601_113521</v>
+      </c>
+      <c r="B545" t="str">
+        <f t="shared" si="20"/>
+        <v>52-24</v>
+      </c>
+      <c r="C545" t="s">
+        <v>235</v>
+      </c>
+      <c r="G545">
+        <v>52</v>
+      </c>
+      <c r="H545">
+        <v>24</v>
+      </c>
+      <c r="K545" t="s">
+        <v>121</v>
+      </c>
+      <c r="L545">
+        <v>113601</v>
+      </c>
+      <c r="M545">
+        <v>113521</v>
+      </c>
+    </row>
+    <row r="546" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A546" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_113521_122521</v>
+      </c>
+      <c r="B546" t="str">
+        <f t="shared" si="20"/>
+        <v>48-26</v>
+      </c>
+      <c r="C546" t="s">
+        <v>235</v>
+      </c>
+      <c r="G546">
+        <v>48</v>
+      </c>
+      <c r="H546">
+        <v>26</v>
+      </c>
+      <c r="K546" t="s">
+        <v>121</v>
+      </c>
+      <c r="L546">
+        <v>113521</v>
+      </c>
+      <c r="M546">
+        <v>122521</v>
+      </c>
+    </row>
+    <row r="547" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A547" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_122521_123321</v>
+      </c>
+      <c r="B547" t="str">
+        <f t="shared" si="20"/>
+        <v>46-28</v>
+      </c>
+      <c r="C547" t="s">
+        <v>235</v>
+      </c>
+      <c r="G547">
+        <v>46</v>
+      </c>
+      <c r="H547">
+        <v>28</v>
+      </c>
+      <c r="K547" t="s">
+        <v>121</v>
+      </c>
+      <c r="L547">
+        <v>122521</v>
+      </c>
+      <c r="M547">
+        <v>123321</v>
+      </c>
+    </row>
+    <row r="548" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A548" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_123321_126021</v>
+      </c>
+      <c r="B548" t="str">
+        <f t="shared" si="20"/>
+        <v>44-29</v>
+      </c>
+      <c r="C548" t="s">
+        <v>235</v>
+      </c>
+      <c r="G548">
+        <v>44</v>
+      </c>
+      <c r="H548">
+        <v>29</v>
+      </c>
+      <c r="K548" t="s">
+        <v>121</v>
+      </c>
+      <c r="L548">
+        <v>123321</v>
+      </c>
+      <c r="M548">
+        <v>126021</v>
+      </c>
+    </row>
+    <row r="549" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A549" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_126021_114602</v>
+      </c>
+      <c r="B549" t="str">
+        <f t="shared" si="20"/>
+        <v>42-29</v>
+      </c>
+      <c r="C549" t="s">
+        <v>235</v>
+      </c>
+      <c r="G549">
+        <v>42</v>
+      </c>
+      <c r="H549">
+        <v>29</v>
+      </c>
+      <c r="K549" t="s">
+        <v>121</v>
+      </c>
+      <c r="L549">
+        <v>126021</v>
+      </c>
+      <c r="M549">
+        <v>114602</v>
+      </c>
+    </row>
+    <row r="550" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A550" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_114602_116822</v>
+      </c>
+      <c r="B550" t="str">
+        <f t="shared" si="20"/>
+        <v>40-29</v>
+      </c>
+      <c r="C550" t="s">
+        <v>235</v>
+      </c>
+      <c r="G550">
+        <v>40</v>
+      </c>
+      <c r="H550">
+        <v>29</v>
+      </c>
+      <c r="K550" t="s">
+        <v>121</v>
+      </c>
+      <c r="L550">
+        <v>114602</v>
+      </c>
+      <c r="M550">
+        <v>116822</v>
+      </c>
+    </row>
+    <row r="551" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A551" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_116822_119322</v>
+      </c>
+      <c r="B551" t="str">
+        <f t="shared" si="20"/>
+        <v>37-28</v>
+      </c>
+      <c r="C551" t="s">
+        <v>235</v>
+      </c>
+      <c r="G551">
+        <v>37</v>
+      </c>
+      <c r="H551">
+        <v>28</v>
+      </c>
+      <c r="K551" t="s">
+        <v>121</v>
+      </c>
+      <c r="L551">
+        <v>116822</v>
+      </c>
+      <c r="M551">
+        <v>119322</v>
+      </c>
+    </row>
+    <row r="552" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A552" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_119322_119402</v>
+      </c>
+      <c r="B552" t="str">
+        <f t="shared" si="20"/>
+        <v>37-26</v>
+      </c>
+      <c r="C552" t="s">
+        <v>235</v>
+      </c>
+      <c r="G552">
+        <v>37</v>
+      </c>
+      <c r="H552">
+        <v>26</v>
+      </c>
+      <c r="K552" t="s">
+        <v>121</v>
+      </c>
+      <c r="L552">
+        <v>119322</v>
+      </c>
+      <c r="M552">
+        <v>119402</v>
+      </c>
+    </row>
+    <row r="553" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A553" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_119402_116022</v>
+      </c>
+      <c r="B553" t="str">
+        <f t="shared" si="20"/>
+        <v>37-22</v>
+      </c>
+      <c r="C553" t="s">
+        <v>235</v>
+      </c>
+      <c r="G553">
+        <v>37</v>
+      </c>
+      <c r="H553">
+        <v>22</v>
+      </c>
+      <c r="K553" t="s">
+        <v>121</v>
+      </c>
+      <c r="L553">
+        <v>119402</v>
+      </c>
+      <c r="M553">
+        <v>116022</v>
+      </c>
+    </row>
+    <row r="554" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A554" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_116022_133002</v>
+      </c>
+      <c r="B554" t="str">
+        <f t="shared" si="20"/>
+        <v>37-20</v>
+      </c>
+      <c r="C554" t="s">
+        <v>235</v>
+      </c>
+      <c r="G554">
+        <v>37</v>
+      </c>
+      <c r="H554">
+        <v>20</v>
+      </c>
+      <c r="K554" t="s">
+        <v>121</v>
+      </c>
+      <c r="L554">
+        <v>116022</v>
+      </c>
+      <c r="M554">
+        <v>133002</v>
+      </c>
+    </row>
+    <row r="555" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A555" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_133002_133102</v>
+      </c>
+      <c r="B555" t="str">
+        <f t="shared" si="20"/>
+        <v>39-15</v>
+      </c>
+      <c r="C555" t="s">
+        <v>235</v>
+      </c>
+      <c r="G555">
+        <v>39</v>
+      </c>
+      <c r="H555">
+        <v>15</v>
+      </c>
+      <c r="K555" t="s">
+        <v>121</v>
+      </c>
+      <c r="L555">
+        <v>133002</v>
+      </c>
+      <c r="M555">
+        <v>133102</v>
+      </c>
+    </row>
+    <row r="556" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A556" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_133102_118002</v>
+      </c>
+      <c r="B556" t="str">
+        <f t="shared" si="20"/>
+        <v>41-13</v>
+      </c>
+      <c r="C556" t="s">
+        <v>235</v>
+      </c>
+      <c r="G556">
+        <v>41</v>
+      </c>
+      <c r="H556">
+        <v>13</v>
+      </c>
+      <c r="K556" t="s">
+        <v>121</v>
+      </c>
+      <c r="L556">
+        <v>133102</v>
+      </c>
+      <c r="M556">
+        <v>118002</v>
+      </c>
+    </row>
+    <row r="557" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A557" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_118002_169302</v>
+      </c>
+      <c r="B557" t="str">
+        <f t="shared" si="20"/>
+        <v>43-11</v>
+      </c>
+      <c r="C557" t="s">
+        <v>235</v>
+      </c>
+      <c r="G557">
+        <v>43</v>
+      </c>
+      <c r="H557">
+        <v>11</v>
+      </c>
+      <c r="K557" t="s">
+        <v>121</v>
+      </c>
+      <c r="L557">
+        <v>118002</v>
+      </c>
+      <c r="M557">
+        <v>169302</v>
+      </c>
+    </row>
+    <row r="558" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A558" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_169302_130202</v>
+      </c>
+      <c r="B558" t="str">
+        <f t="shared" si="20"/>
+        <v>45-9</v>
+      </c>
+      <c r="C558" t="s">
+        <v>235</v>
+      </c>
+      <c r="G558">
+        <v>45</v>
+      </c>
+      <c r="H558">
+        <v>9</v>
+      </c>
+      <c r="K558" t="s">
+        <v>121</v>
+      </c>
+      <c r="L558">
+        <v>169302</v>
+      </c>
+      <c r="M558">
+        <v>130202</v>
+      </c>
+    </row>
+    <row r="559" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A559" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_130202_130402</v>
+      </c>
+      <c r="B559" t="str">
+        <f t="shared" si="20"/>
+        <v>47-7</v>
+      </c>
+      <c r="C559" t="s">
+        <v>235</v>
+      </c>
+      <c r="G559">
+        <v>47</v>
+      </c>
+      <c r="H559">
+        <v>7</v>
+      </c>
+      <c r="K559" t="s">
+        <v>121</v>
+      </c>
+      <c r="L559">
+        <v>130202</v>
+      </c>
+      <c r="M559">
+        <v>130402</v>
+      </c>
+    </row>
+    <row r="560" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A560" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_130402_61901</v>
+      </c>
+      <c r="B560" t="str">
+        <f t="shared" si="20"/>
+        <v>49-5</v>
+      </c>
+      <c r="C560" t="s">
+        <v>235</v>
+      </c>
+      <c r="D560" t="s">
+        <v>241</v>
+      </c>
+      <c r="G560">
+        <v>49</v>
+      </c>
+      <c r="H560">
+        <v>5</v>
+      </c>
+      <c r="K560" t="s">
+        <v>121</v>
+      </c>
+      <c r="L560">
+        <v>130402</v>
+      </c>
+      <c r="M560">
+        <v>61901</v>
+      </c>
+    </row>
+    <row r="561" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A561" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_61902_130401</v>
+      </c>
+      <c r="B561" t="str">
+        <f t="shared" si="20"/>
+        <v>49-2</v>
+      </c>
+      <c r="C561" t="s">
+        <v>236</v>
+      </c>
+      <c r="D561" t="s">
+        <v>242</v>
+      </c>
+      <c r="G561">
+        <v>49</v>
+      </c>
+      <c r="H561">
+        <v>2</v>
+      </c>
+      <c r="K561" t="s">
+        <v>121</v>
+      </c>
+      <c r="L561">
+        <v>61902</v>
+      </c>
+      <c r="M561">
+        <v>130401</v>
+      </c>
+    </row>
+    <row r="562" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A562" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_130401_130201</v>
+      </c>
+      <c r="B562" t="str">
+        <f t="shared" si="20"/>
+        <v>48-4</v>
+      </c>
+      <c r="C562" t="s">
+        <v>236</v>
+      </c>
+      <c r="G562">
+        <v>48</v>
+      </c>
+      <c r="H562">
+        <v>4</v>
+      </c>
+      <c r="K562" t="s">
+        <v>121</v>
+      </c>
+      <c r="L562">
+        <v>130401</v>
+      </c>
+      <c r="M562">
+        <v>130201</v>
+      </c>
+    </row>
+    <row r="563" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A563" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_130201_169301</v>
+      </c>
+      <c r="B563" t="str">
+        <f t="shared" si="20"/>
+        <v>46-6</v>
+      </c>
+      <c r="C563" t="s">
+        <v>236</v>
+      </c>
+      <c r="G563">
+        <v>46</v>
+      </c>
+      <c r="H563">
+        <v>6</v>
+      </c>
+      <c r="K563" t="s">
+        <v>121</v>
+      </c>
+      <c r="L563">
+        <v>130201</v>
+      </c>
+      <c r="M563">
+        <v>169301</v>
+      </c>
+    </row>
+    <row r="564" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A564" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_169301_118001</v>
+      </c>
+      <c r="B564" t="str">
+        <f t="shared" si="20"/>
+        <v>44-8</v>
+      </c>
+      <c r="C564" t="s">
+        <v>236</v>
+      </c>
+      <c r="G564">
+        <v>44</v>
+      </c>
+      <c r="H564">
+        <v>8</v>
+      </c>
+      <c r="K564" t="s">
+        <v>121</v>
+      </c>
+      <c r="L564">
+        <v>169301</v>
+      </c>
+      <c r="M564">
+        <v>118001</v>
+      </c>
+    </row>
+    <row r="565" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A565" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_118001_133101</v>
+      </c>
+      <c r="B565" t="str">
+        <f t="shared" si="20"/>
+        <v>42-10</v>
+      </c>
+      <c r="C565" t="s">
+        <v>236</v>
+      </c>
+      <c r="G565">
+        <v>42</v>
+      </c>
+      <c r="H565">
+        <v>10</v>
+      </c>
+      <c r="K565" t="s">
+        <v>121</v>
+      </c>
+      <c r="L565">
+        <v>118001</v>
+      </c>
+      <c r="M565">
+        <v>133101</v>
+      </c>
+    </row>
+    <row r="566" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A566" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_133101_133001</v>
+      </c>
+      <c r="B566" t="str">
+        <f t="shared" si="20"/>
+        <v>40-12</v>
+      </c>
+      <c r="C566" t="s">
+        <v>236</v>
+      </c>
+      <c r="G566">
+        <v>40</v>
+      </c>
+      <c r="H566">
+        <v>12</v>
+      </c>
+      <c r="K566" t="s">
+        <v>121</v>
+      </c>
+      <c r="L566">
+        <v>133101</v>
+      </c>
+      <c r="M566">
+        <v>133001</v>
+      </c>
+    </row>
+    <row r="567" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A567" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_133001_116021</v>
+      </c>
+      <c r="B567" t="str">
+        <f t="shared" si="20"/>
+        <v>38-14</v>
+      </c>
+      <c r="C567" t="s">
+        <v>236</v>
+      </c>
+      <c r="G567">
+        <v>38</v>
+      </c>
+      <c r="H567">
+        <v>14</v>
+      </c>
+      <c r="K567" t="s">
+        <v>121</v>
+      </c>
+      <c r="L567">
+        <v>133001</v>
+      </c>
+      <c r="M567">
+        <v>116021</v>
+      </c>
+    </row>
+    <row r="568" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A568" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_116021_119421</v>
+      </c>
+      <c r="B568" t="str">
+        <f t="shared" si="20"/>
+        <v>36-20</v>
+      </c>
+      <c r="C568" t="s">
+        <v>236</v>
+      </c>
+      <c r="G568">
+        <v>36</v>
+      </c>
+      <c r="H568">
+        <v>20</v>
+      </c>
+      <c r="K568" t="s">
+        <v>121</v>
+      </c>
+      <c r="L568">
+        <v>116021</v>
+      </c>
+      <c r="M568">
+        <v>119421</v>
+      </c>
+    </row>
+    <row r="569" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A569" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_119421_119321</v>
+      </c>
+      <c r="B569" t="str">
+        <f t="shared" si="20"/>
+        <v>36-22</v>
+      </c>
+      <c r="C569" t="s">
+        <v>236</v>
+      </c>
+      <c r="G569">
+        <v>36</v>
+      </c>
+      <c r="H569">
+        <v>22</v>
+      </c>
+      <c r="K569" t="s">
+        <v>121</v>
+      </c>
+      <c r="L569">
+        <v>119421</v>
+      </c>
+      <c r="M569">
+        <v>119321</v>
+      </c>
+    </row>
+    <row r="570" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A570" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_119321_116821</v>
+      </c>
+      <c r="B570" t="str">
+        <f t="shared" si="20"/>
+        <v>36-26</v>
+      </c>
+      <c r="C570" t="s">
+        <v>236</v>
+      </c>
+      <c r="G570">
+        <v>36</v>
+      </c>
+      <c r="H570">
+        <v>26</v>
+      </c>
+      <c r="K570" t="s">
+        <v>121</v>
+      </c>
+      <c r="L570">
+        <v>119321</v>
+      </c>
+      <c r="M570">
+        <v>116821</v>
+      </c>
+    </row>
+    <row r="571" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A571" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_116821_114601</v>
+      </c>
+      <c r="B571" t="str">
+        <f t="shared" si="20"/>
+        <v>36-28</v>
+      </c>
+      <c r="C571" t="s">
+        <v>236</v>
+      </c>
+      <c r="G571">
+        <v>36</v>
+      </c>
+      <c r="H571">
+        <v>28</v>
+      </c>
+      <c r="K571" t="s">
+        <v>121</v>
+      </c>
+      <c r="L571">
+        <v>116821</v>
+      </c>
+      <c r="M571">
+        <v>114601</v>
+      </c>
+    </row>
+    <row r="572" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A572" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_114601_126022</v>
+      </c>
+      <c r="B572" t="str">
+        <f t="shared" si="20"/>
+        <v>40-30</v>
+      </c>
+      <c r="C572" t="s">
+        <v>236</v>
+      </c>
+      <c r="G572">
+        <v>40</v>
+      </c>
+      <c r="H572">
+        <v>30</v>
+      </c>
+      <c r="K572" t="s">
+        <v>121</v>
+      </c>
+      <c r="L572">
+        <v>114601</v>
+      </c>
+      <c r="M572">
+        <v>126022</v>
+      </c>
+    </row>
+    <row r="573" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A573" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_126022_123322</v>
+      </c>
+      <c r="B573" t="str">
+        <f t="shared" si="20"/>
+        <v>42-30</v>
+      </c>
+      <c r="C573" t="s">
+        <v>236</v>
+      </c>
+      <c r="G573">
+        <v>42</v>
+      </c>
+      <c r="H573">
+        <v>30</v>
+      </c>
+      <c r="K573" t="s">
+        <v>121</v>
+      </c>
+      <c r="L573">
+        <v>126022</v>
+      </c>
+      <c r="M573">
+        <v>123322</v>
+      </c>
+    </row>
+    <row r="574" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A574" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_123322_122522</v>
+      </c>
+      <c r="B574" t="str">
+        <f t="shared" si="20"/>
+        <v>44-30</v>
+      </c>
+      <c r="C574" t="s">
+        <v>236</v>
+      </c>
+      <c r="G574">
+        <v>44</v>
+      </c>
+      <c r="H574">
+        <v>30</v>
+      </c>
+      <c r="K574" t="s">
+        <v>121</v>
+      </c>
+      <c r="L574">
+        <v>123322</v>
+      </c>
+      <c r="M574">
+        <v>122522</v>
+      </c>
+    </row>
+    <row r="575" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A575" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_122522_113522</v>
+      </c>
+      <c r="B575" t="str">
+        <f t="shared" si="20"/>
+        <v>47-29</v>
+      </c>
+      <c r="C575" t="s">
+        <v>236</v>
+      </c>
+      <c r="G575">
+        <v>47</v>
+      </c>
+      <c r="H575">
+        <v>29</v>
+      </c>
+      <c r="K575" t="s">
+        <v>121</v>
+      </c>
+      <c r="L575">
+        <v>122522</v>
+      </c>
+      <c r="M575">
+        <v>113522</v>
+      </c>
+    </row>
+    <row r="576" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A576" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_113522_113602</v>
+      </c>
+      <c r="B576" t="str">
+        <f t="shared" si="20"/>
+        <v>49-27</v>
+      </c>
+      <c r="C576" t="s">
+        <v>236</v>
+      </c>
+      <c r="G576">
+        <v>49</v>
+      </c>
+      <c r="H576">
+        <v>27</v>
+      </c>
+      <c r="K576" t="s">
+        <v>121</v>
+      </c>
+      <c r="L576">
+        <v>113522</v>
+      </c>
+      <c r="M576">
+        <v>113602</v>
+      </c>
+    </row>
+    <row r="577" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A577" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_113602_113302</v>
+      </c>
+      <c r="B577" t="str">
+        <f t="shared" si="20"/>
+        <v>52-25</v>
+      </c>
+      <c r="C577" t="s">
+        <v>236</v>
+      </c>
+      <c r="G577">
+        <v>52</v>
+      </c>
+      <c r="H577">
+        <v>25</v>
+      </c>
+      <c r="K577" t="s">
+        <v>121</v>
+      </c>
+      <c r="L577">
+        <v>113602</v>
+      </c>
+      <c r="M577">
+        <v>113302</v>
+      </c>
+    </row>
+    <row r="578" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A578" t="str">
+        <f t="shared" si="19"/>
+        <v>DEPOT_113302_51602</v>
+      </c>
+      <c r="B578" t="str">
+        <f t="shared" si="20"/>
+        <v>56-25</v>
+      </c>
+      <c r="C578" t="s">
+        <v>236</v>
+      </c>
+      <c r="G578">
+        <v>56</v>
+      </c>
+      <c r="H578">
+        <v>25</v>
+      </c>
+      <c r="K578" t="s">
+        <v>121</v>
+      </c>
+      <c r="L578">
+        <v>113302</v>
+      </c>
+      <c r="M578">
+        <v>51602</v>
+      </c>
+    </row>
+    <row r="579" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A579" t="str">
+        <f t="shared" ref="A579:A580" si="21">_xlfn.CONCAT(K579,"_",L579,"_",M579)</f>
+        <v>DEPOT_51602_51502</v>
+      </c>
+      <c r="B579" t="str">
+        <f t="shared" si="20"/>
+        <v>58-25</v>
+      </c>
+      <c r="C579" t="s">
+        <v>236</v>
+      </c>
+      <c r="G579">
+        <v>58</v>
+      </c>
+      <c r="H579">
+        <v>25</v>
+      </c>
+      <c r="K579" t="s">
+        <v>121</v>
+      </c>
+      <c r="L579">
+        <v>51602</v>
+      </c>
+      <c r="M579">
+        <v>51502</v>
+      </c>
+    </row>
+    <row r="580" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A580" t="str">
+        <f t="shared" si="21"/>
+        <v>DEPOT_51502_574202</v>
+      </c>
+      <c r="B580" t="str">
+        <f t="shared" si="20"/>
+        <v>60-25</v>
+      </c>
+      <c r="C580" t="s">
+        <v>236</v>
+      </c>
+      <c r="D580" t="s">
+        <v>240</v>
+      </c>
+      <c r="G580">
+        <v>60</v>
+      </c>
+      <c r="H580">
+        <v>25</v>
+      </c>
+      <c r="K580" t="s">
+        <v>121</v>
+      </c>
+      <c r="L580">
+        <v>51502</v>
+      </c>
+      <c r="M580">
+        <v>574202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>